<commit_message>
updates output files to have multiple unique elements in a single file and has GUI able to display different elements at once
</commit_message>
<xml_diff>
--- a/runs/run708/NotionalETEOutput708.xlsx
+++ b/runs/run708/NotionalETEOutput708.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="17">
   <si>
     <t>uniqueid</t>
   </si>
@@ -49,13 +49,22 @@
     <t>tUp</t>
   </si>
   <si>
-    <t>Missile_HIGHWIND3_State_Update</t>
+    <t>Missile_BRAVER_State_Update</t>
   </si>
   <si>
-    <t>MISSILE_HIGHWIND3_54.MISSILE_HIGHWIND3_54</t>
+    <t>Missile_HIGHWIND_State_Update</t>
   </si>
   <si>
-    <t>MISSILE_HIGHWIND3</t>
+    <t>MISSILE_BRAVER_259.MISSILE_BRAVER_259</t>
+  </si>
+  <si>
+    <t>MISSILE_HIGHWIND_26.MISSILE_HIGHWIND_26</t>
+  </si>
+  <si>
+    <t>MISSILE_BRAVER</t>
+  </si>
+  <si>
+    <t>MISSILE_HIGHWIND</t>
   </si>
 </sst>
 </file>
@@ -413,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,28 +471,28 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>152.142</v>
       </c>
       <c r="F2">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G2">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H2">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I2">
-        <v>-1162.105522252194</v>
+        <v>-1828.955776444838</v>
       </c>
       <c r="J2">
-        <v>2546.842399320076</v>
+        <v>2276.952653270968</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -497,31 +506,31 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>153.142</v>
       </c>
       <c r="F3">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G3">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H3">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I3">
-        <v>-1139.162464861196</v>
+        <v>-1792.84731938902</v>
       </c>
       <c r="J3">
-        <v>2484.888435464121</v>
+        <v>2221.563971811868</v>
       </c>
       <c r="K3">
-        <v>484.9425215140221</v>
+        <v>267.8456407079808</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -532,31 +541,31 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>154.142</v>
       </c>
       <c r="F4">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G4">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H4">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I4">
-        <v>-1115.65445578917</v>
+        <v>-1755.849724797375</v>
       </c>
       <c r="J4">
-        <v>2422.934471608167</v>
+        <v>2166.175290352768</v>
       </c>
       <c r="K4">
-        <v>945.703586008638</v>
+        <v>522.3352700099211</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -567,31 +576,31 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>155.142</v>
       </c>
       <c r="F5">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G5">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H5">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I5">
-        <v>-1091.567583620718</v>
+        <v>-1717.941098476073</v>
       </c>
       <c r="J5">
-        <v>2360.980507752213</v>
+        <v>2110.786608893668</v>
       </c>
       <c r="K5">
-        <v>1382.283193483851</v>
+        <v>763.4688879058228</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -602,31 +611,31 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>156.142</v>
       </c>
       <c r="F6">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G6">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H6">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I6">
-        <v>-1066.887594384633</v>
+        <v>-1679.099007106906</v>
       </c>
       <c r="J6">
-        <v>2299.026543896258</v>
+        <v>2055.397927434569</v>
       </c>
       <c r="K6">
-        <v>1794.681343939659</v>
+        <v>991.2464943956843</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -637,31 +646,31 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>157.142</v>
       </c>
       <c r="F7">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G7">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H7">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I7">
-        <v>-1041.599883118784</v>
+        <v>-1639.300464971841</v>
       </c>
       <c r="J7">
-        <v>2237.072580040304</v>
+        <v>2000.009245975469</v>
       </c>
       <c r="K7">
-        <v>2182.898037376065</v>
+        <v>1205.668089479507</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -672,31 +681,31 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>158.142</v>
       </c>
       <c r="F8">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G8">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H8">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I8">
-        <v>-1015.68948522728</v>
+        <v>-1598.521920350689</v>
       </c>
       <c r="J8">
-        <v>2175.118616184349</v>
+        <v>1944.620564516369</v>
       </c>
       <c r="K8">
-        <v>2546.933273793065</v>
+        <v>1406.733673157291</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -707,31 +716,31 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>159.142</v>
       </c>
       <c r="F9">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G9">
-        <v>-77.45070893424069</v>
+        <v>-63.60849505983672</v>
       </c>
       <c r="H9">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I9">
-        <v>-989.1410676248275</v>
+        <v>-1556.739241583813</v>
       </c>
       <c r="J9">
-        <v>2113.164652328395</v>
+        <v>1889.231883057269</v>
       </c>
       <c r="K9">
-        <v>2886.787053190662</v>
+        <v>1594.443245429035</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -742,31 +751,31 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>160.142</v>
       </c>
       <c r="F10">
-        <v>143.5549374721454</v>
+        <v>281.8416054706128</v>
       </c>
       <c r="G10">
-        <v>-64.66141679516831</v>
+        <v>-53.10494206411526</v>
       </c>
       <c r="H10">
-        <v>1218.959915217622</v>
+        <v>445.1400166036313</v>
       </c>
       <c r="I10">
-        <v>-961.938919663011</v>
+        <v>-1513.927702791663</v>
       </c>
       <c r="J10">
-        <v>2051.210688472441</v>
+        <v>1833.84320159817</v>
       </c>
       <c r="K10">
-        <v>3202.459375568853</v>
+        <v>1768.796806294738</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -777,31 +786,31 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>161.142</v>
       </c>
       <c r="F11">
-        <v>111.4153780890127</v>
+        <v>218.7419644887912</v>
       </c>
       <c r="G11">
-        <v>-51.87212465609592</v>
+        <v>-42.6013890683938</v>
       </c>
       <c r="H11">
-        <v>1501.750413098804</v>
+        <v>548.4095050836562</v>
       </c>
       <c r="I11">
-        <v>-934.0669438331518</v>
+        <v>-1470.06196924265</v>
       </c>
       <c r="J11">
-        <v>1989.256724616487</v>
+        <v>1778.45452013907</v>
       </c>
       <c r="K11">
-        <v>3493.95024092764</v>
+        <v>1929.794355754402</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -812,31 +821,31 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>162.142</v>
       </c>
       <c r="F12">
-        <v>92.53499924576516</v>
+        <v>181.674090831664</v>
       </c>
       <c r="G12">
-        <v>-39.08283251702354</v>
+        <v>-32.09783607267235</v>
       </c>
       <c r="H12">
-        <v>1670.194896091953</v>
+        <v>609.9220938245039</v>
       </c>
       <c r="I12">
-        <v>-905.5086462402301</v>
+        <v>-1425.116082360727</v>
       </c>
       <c r="J12">
-        <v>1927.302760760532</v>
+        <v>1723.06583867997</v>
       </c>
       <c r="K12">
-        <v>3761.259649267024</v>
+        <v>2077.435893808028</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -847,31 +856,31 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <v>163.142</v>
       </c>
       <c r="F13">
-        <v>80.61631898523416</v>
+        <v>158.2741295424833</v>
       </c>
       <c r="G13">
-        <v>-26.29354037795115</v>
+        <v>-21.59428307695089</v>
       </c>
       <c r="H13">
-        <v>1790.57078335978</v>
+        <v>653.880983520652</v>
       </c>
       <c r="I13">
-        <v>-876.247126842234</v>
+        <v>-1379.063444363793</v>
       </c>
       <c r="J13">
-        <v>1865.348796904578</v>
+        <v>1667.67715722087</v>
       </c>
       <c r="K13">
-        <v>4004.387600587004</v>
+        <v>2211.721420455614</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -882,31 +891,31 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <v>164.142</v>
       </c>
       <c r="F14">
-        <v>72.30427975230334</v>
+        <v>141.955091525428</v>
       </c>
       <c r="G14">
-        <v>-13.50424823887876</v>
+        <v>-11.09073008122943</v>
       </c>
       <c r="H14">
-        <v>1884.307422283808</v>
+        <v>688.1117473760502</v>
       </c>
       <c r="I14">
-        <v>-846.2650694491671</v>
+        <v>-1331.876802523836</v>
       </c>
       <c r="J14">
-        <v>1803.394833048623</v>
+        <v>1612.288475761771</v>
       </c>
       <c r="K14">
-        <v>4223.33409488758</v>
+        <v>2332.650935697161</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -917,31 +926,31 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <v>165.142</v>
       </c>
       <c r="F15">
-        <v>66.10324956736265</v>
+        <v>129.7806004652753</v>
       </c>
       <c r="G15">
-        <v>-0.7149560998063795</v>
+        <v>-0.5871770855079788</v>
       </c>
       <c r="H15">
-        <v>1961.085000439055</v>
+        <v>716.14939815369</v>
       </c>
       <c r="I15">
-        <v>-815.5447314757829</v>
+        <v>-1283.528233039485</v>
       </c>
       <c r="J15">
-        <v>1741.440869192669</v>
+        <v>1556.899794302671</v>
       </c>
       <c r="K15">
-        <v>4418.099132168751</v>
+        <v>2440.224439532667</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -952,31 +961,31 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <v>166.142</v>
       </c>
       <c r="F16">
-        <v>61.25490991093175</v>
+        <v>120.2618485735093</v>
       </c>
       <c r="G16">
-        <v>12.07433603926601</v>
+        <v>9.916375910213482</v>
       </c>
       <c r="H16">
-        <v>2026.110004644981</v>
+        <v>739.8952417130405</v>
       </c>
       <c r="I16">
-        <v>-784.0679334419968</v>
+        <v>-1233.98912451145</v>
       </c>
       <c r="J16">
-        <v>1679.486905336714</v>
+        <v>1501.511112843571</v>
       </c>
       <c r="K16">
-        <v>4588.682712430517</v>
+        <v>2534.441931962135</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -987,31 +996,31 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>167.142</v>
       </c>
       <c r="F17">
-        <v>57.33225010969327</v>
+        <v>112.5604852100193</v>
       </c>
       <c r="G17">
-        <v>24.8636281783384</v>
+        <v>20.41992890593494</v>
       </c>
       <c r="H17">
-        <v>2082.507352975426</v>
+        <v>760.4904362381479</v>
       </c>
       <c r="I17">
-        <v>-751.8160482147517</v>
+        <v>-1183.230161011056</v>
       </c>
       <c r="J17">
-        <v>1617.53294148076</v>
+        <v>1446.122431384472</v>
       </c>
       <c r="K17">
-        <v>4735.08483567288</v>
+        <v>2615.303412985563</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1022,31 +1031,31 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>168.142</v>
       </c>
       <c r="F18">
-        <v>54.07504475267618</v>
+        <v>106.1656094688257</v>
       </c>
       <c r="G18">
-        <v>37.65292031741078</v>
+        <v>30.92348190165639</v>
       </c>
       <c r="H18">
-        <v>2132.300630825009</v>
+        <v>778.6739550331488</v>
       </c>
       <c r="I18">
-        <v>-718.7699899849764</v>
+        <v>-1131.221304731855</v>
       </c>
       <c r="J18">
-        <v>1555.578977624805</v>
+        <v>1390.733749925372</v>
       </c>
       <c r="K18">
-        <v>4857.305501895839</v>
+        <v>2682.808882602952</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1057,31 +1066,31 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>169.142</v>
       </c>
       <c r="F19">
-        <v>51.31480828685667</v>
+        <v>100.74643343278</v>
       </c>
       <c r="G19">
-        <v>50.44221245648318</v>
+        <v>41.42703489737787</v>
       </c>
       <c r="H19">
-        <v>2176.875634345856</v>
+        <v>794.9518634037736</v>
       </c>
       <c r="I19">
-        <v>-684.9102029731087</v>
+        <v>-1077.931778214048</v>
       </c>
       <c r="J19">
-        <v>1493.625013768851</v>
+        <v>1335.345068466272</v>
       </c>
       <c r="K19">
-        <v>4955.344711099394</v>
+        <v>2736.958340814301</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1092,31 +1101,31 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E20">
         <v>170.142</v>
       </c>
       <c r="F20">
-        <v>48.93713386123383</v>
+        <v>96.07834197452561</v>
       </c>
       <c r="G20">
-        <v>63.23150459555556</v>
+        <v>51.93058789309931</v>
       </c>
       <c r="H20">
-        <v>2217.223092046545</v>
+        <v>809.6859557775927</v>
       </c>
       <c r="I20">
-        <v>-650.2166498565065</v>
+        <v>-1023.330046131206</v>
       </c>
       <c r="J20">
-        <v>1431.671049912897</v>
+        <v>1279.956387007172</v>
       </c>
       <c r="K20">
-        <v>5029.202463283545</v>
+        <v>2777.751787619611</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1127,31 +1136,31 @@
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E21">
         <v>171.142</v>
       </c>
       <c r="F21">
-        <v>46.8613012291037</v>
+        <v>92.00285692308762</v>
       </c>
       <c r="G21">
-        <v>76.02079673462794</v>
+        <v>62.43414088882076</v>
       </c>
       <c r="H21">
-        <v>2254.075887696693</v>
+        <v>823.1438667907438</v>
       </c>
       <c r="I21">
-        <v>-614.6687999118918</v>
+        <v>-967.3837966284975</v>
       </c>
       <c r="J21">
-        <v>1369.717086056942</v>
+        <v>1224.567705548072</v>
       </c>
       <c r="K21">
-        <v>5078.878758448291</v>
+        <v>2805.189223018881</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1162,31 +1171,31 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E22">
         <v>172.142</v>
       </c>
       <c r="F22">
-        <v>45.02853721144141</v>
+        <v>88.40458881554213</v>
       </c>
       <c r="G22">
-        <v>88.81008887370034</v>
+        <v>72.93769388454224</v>
       </c>
       <c r="H22">
-        <v>2287.991435899885</v>
+        <v>835.5291532155192</v>
       </c>
       <c r="I22">
-        <v>-578.2456168658131</v>
+        <v>-910.0599222013897</v>
       </c>
       <c r="J22">
-        <v>1307.763122200988</v>
+        <v>1169.179024088973</v>
       </c>
       <c r="K22">
-        <v>5104.373596593632</v>
+        <v>2819.270647012112</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1197,31 +1206,31 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E23">
         <v>173.142</v>
       </c>
       <c r="F23">
-        <v>43.39490864239923</v>
+        <v>85.19728360717305</v>
       </c>
       <c r="G23">
-        <v>101.5993810127727</v>
+        <v>83.44124688026369</v>
       </c>
       <c r="H23">
-        <v>2319.403580622833</v>
+        <v>847.0002462752382</v>
       </c>
       <c r="I23">
-        <v>-540.9255464459386</v>
+        <v>-851.3245001035117</v>
       </c>
       <c r="J23">
-        <v>1245.809158345033</v>
+        <v>1113.790342629873</v>
       </c>
       <c r="K23">
-        <v>5105.68697771957</v>
+        <v>2819.996059599303</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1232,31 +1241,31 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>174.142</v>
       </c>
       <c r="F24">
-        <v>41.92683537578966</v>
+        <v>82.31501335095138</v>
       </c>
       <c r="G24">
-        <v>114.3886731518451</v>
+        <v>93.94479987598515</v>
       </c>
       <c r="H24">
-        <v>2348.656620291432</v>
+        <v>857.6828769353795</v>
       </c>
       <c r="I24">
-        <v>-502.6865036258101</v>
+        <v>-791.1427722720713</v>
       </c>
       <c r="J24">
-        <v>1183.855194489079</v>
+        <v>1058.401661170773</v>
       </c>
       <c r="K24">
-        <v>5082.818901826104</v>
+        <v>2807.365460780455</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1267,31 +1276,31 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E25">
         <v>175.142</v>
       </c>
       <c r="F25">
-        <v>40.598155027322</v>
+        <v>79.70641340194551</v>
       </c>
       <c r="G25">
-        <v>127.1779652909175</v>
+        <v>104.4483528717066</v>
       </c>
       <c r="H25">
-        <v>2376.028372381528</v>
+        <v>867.6784986352782</v>
       </c>
       <c r="I25">
-        <v>-463.50585955551</v>
+        <v>-729.4791247589554</v>
       </c>
       <c r="J25">
-        <v>1121.901230633125</v>
+        <v>1003.012979711674</v>
       </c>
       <c r="K25">
-        <v>5035.769368913234</v>
+        <v>2781.378850555568</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1302,31 +1311,31 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E26">
         <v>176.142</v>
       </c>
       <c r="F26">
-        <v>39.38814347686456</v>
+        <v>77.33079606670002</v>
       </c>
       <c r="G26">
-        <v>139.9672574299899</v>
+        <v>114.9519058674281</v>
       </c>
       <c r="H26">
-        <v>2401.746259112866</v>
+        <v>877.0701614649408</v>
       </c>
       <c r="I26">
-        <v>-423.3604281705104</v>
+        <v>-666.297066655345</v>
       </c>
       <c r="J26">
-        <v>1059.94726677717</v>
+        <v>947.6242982525737</v>
       </c>
       <c r="K26">
-        <v>4964.538378980958</v>
+        <v>2742.03622892464</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1337,31 +1346,31 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E27">
         <v>177.142</v>
       </c>
       <c r="F27">
-        <v>38.28014425664625</v>
+        <v>75.15545967921346</v>
       </c>
       <c r="G27">
-        <v>152.7565495690623</v>
+        <v>125.4554588631495</v>
       </c>
       <c r="H27">
-        <v>2425.998804303983</v>
+        <v>885.9267105887295</v>
       </c>
       <c r="I27">
-        <v>-382.226452470775</v>
+        <v>-601.5592084973608</v>
       </c>
       <c r="J27">
-        <v>997.9933029212158</v>
+        <v>892.2356167934739</v>
       </c>
       <c r="K27">
-        <v>4869.12593202928</v>
+        <v>2689.337595887674</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1372,31 +1381,31 @@
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E28">
         <v>178.142</v>
       </c>
       <c r="F28">
-        <v>37.26059739639257</v>
+        <v>73.15378193126296</v>
       </c>
       <c r="G28">
-        <v>165.5458417081346</v>
+        <v>135.959011858871</v>
       </c>
       <c r="H28">
-        <v>2448.94402785081</v>
+        <v>894.3058517426738</v>
       </c>
       <c r="I28">
-        <v>-340.0795904619976</v>
+        <v>-535.227240139974</v>
       </c>
       <c r="J28">
-        <v>936.0393390652616</v>
+        <v>836.8469353343743</v>
       </c>
       <c r="K28">
-        <v>4749.532028058197</v>
+        <v>2623.282951444668</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1407,31 +1416,31 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E29">
         <v>179.142</v>
       </c>
       <c r="F29">
-        <v>36.31833716859911</v>
+        <v>71.30384113473728</v>
       </c>
       <c r="G29">
-        <v>178.3351338472071</v>
+        <v>146.4625648545924</v>
       </c>
       <c r="H29">
-        <v>2470.715691189996</v>
+        <v>902.2564319539712</v>
       </c>
       <c r="I29">
-        <v>-296.8949007506556</v>
+        <v>-467.2619080860777</v>
       </c>
       <c r="J29">
-        <v>874.085375209307</v>
+        <v>781.4582538752744</v>
       </c>
       <c r="K29">
-        <v>4605.75666706771</v>
+        <v>2543.872295595623</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1442,31 +1451,31 @@
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E30">
         <v>180.142</v>
       </c>
       <c r="F30">
-        <v>35.44407502001914</v>
+        <v>69.58740106031786</v>
       </c>
       <c r="G30">
-        <v>191.1244259862794</v>
+        <v>156.9661178503139</v>
       </c>
       <c r="H30">
-        <v>2491.428021900982</v>
+        <v>909.8201648720811</v>
       </c>
       <c r="I30">
-        <v>-252.6468277843579</v>
+        <v>-397.6229922573134</v>
       </c>
       <c r="J30">
-        <v>812.1314113533525</v>
+        <v>726.0695724161747</v>
       </c>
       <c r="K30">
-        <v>4437.799849057818</v>
+        <v>2451.105628340538</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1477,31 +1486,31 @@
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E31">
         <v>181.142</v>
       </c>
       <c r="F31">
-        <v>34.63001265291826</v>
+        <v>67.98915129937572</v>
       </c>
       <c r="G31">
-        <v>203.9137181253518</v>
+        <v>167.4696708460353</v>
       </c>
       <c r="H31">
-        <v>2511.179341305285</v>
+        <v>917.0329554961318</v>
       </c>
       <c r="I31">
-        <v>-207.309186728746</v>
+        <v>-326.2692821928938</v>
       </c>
       <c r="J31">
-        <v>750.1774474973984</v>
+        <v>670.680890957075</v>
       </c>
       <c r="K31">
-        <v>4245.661574028523</v>
+        <v>2344.982949679414</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1512,31 +1521,31 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <v>182.142</v>
       </c>
       <c r="F32">
-        <v>33.86954825641904</v>
+        <v>66.49613050756791</v>
       </c>
       <c r="G32">
-        <v>216.7030102644242</v>
+        <v>177.9732238417568</v>
       </c>
       <c r="H32">
-        <v>2530.054887201562</v>
+        <v>923.9259309818523</v>
       </c>
       <c r="I32">
-        <v>-160.8551479720046</v>
+        <v>-253.1585526623474</v>
       </c>
       <c r="J32">
-        <v>688.2234836414439</v>
+        <v>615.2922094979751</v>
       </c>
       <c r="K32">
-        <v>4029.341841979823</v>
+        <v>2225.50425961225</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1547,31 +1556,31 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E33">
         <v>183.142</v>
       </c>
       <c r="F33">
-        <v>33.15705050994647</v>
+        <v>65.09728270549225</v>
       </c>
       <c r="G33">
-        <v>229.4923024034966</v>
+        <v>188.4767768374782</v>
       </c>
       <c r="H33">
-        <v>2548.129036954672</v>
+        <v>930.5262524696675</v>
       </c>
       <c r="I33">
-        <v>-113.2572212478102</v>
+        <v>-178.2475386777488</v>
       </c>
       <c r="J33">
-        <v>626.2695197854896</v>
+        <v>559.9035280388756</v>
       </c>
       <c r="K33">
-        <v>3788.84065291172</v>
+        <v>2092.669558139048</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1582,31 +1591,31 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E34">
         <v>184.142</v>
       </c>
       <c r="F34">
-        <v>32.48768263371084</v>
+        <v>63.78311183675907</v>
       </c>
       <c r="G34">
-        <v>242.281594542569</v>
+        <v>198.9803298331997</v>
       </c>
       <c r="H34">
-        <v>2565.467077591514</v>
+        <v>936.8577614886333</v>
       </c>
       <c r="I34">
-        <v>-64.48723936732212</v>
+        <v>-101.4919098906485</v>
       </c>
       <c r="J34">
-        <v>564.3155559295351</v>
+        <v>504.5148465797757</v>
       </c>
       <c r="K34">
-        <v>3524.158006824212</v>
+        <v>1946.478845259805</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1617,31 +1626,31 @@
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E35">
         <v>185.142</v>
       </c>
       <c r="F35">
-        <v>31.85726390088611</v>
+        <v>62.54540987466149</v>
       </c>
       <c r="G35">
-        <v>255.0708866816414</v>
+        <v>209.4838828289212</v>
       </c>
       <c r="H35">
-        <v>2582.12662934615</v>
+        <v>942.9414998069223</v>
       </c>
       <c r="I35">
-        <v>-14.51634155058785</v>
+        <v>-22.84624435854989</v>
       </c>
       <c r="J35">
-        <v>502.3615920735806</v>
+        <v>449.1261651206759</v>
       </c>
       <c r="K35">
-        <v>3235.293903717299</v>
+        <v>1786.932120974522</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1652,31 +1661,31 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E36">
         <v>186.142</v>
       </c>
       <c r="F36">
-        <v>31.26215954036103</v>
+        <v>61.37704066809557</v>
       </c>
       <c r="G36">
-        <v>267.8601788207138</v>
+        <v>219.9874358246427</v>
       </c>
       <c r="H36">
-        <v>2598.158801013149</v>
+        <v>948.7961313439782</v>
       </c>
       <c r="I36">
-        <v>36.68504365250062</v>
+        <v>57.73599833459129</v>
       </c>
       <c r="J36">
-        <v>440.4076282176264</v>
+        <v>393.7374836615763</v>
       </c>
       <c r="K36">
-        <v>2922.248343590983</v>
+        <v>1614.029385283201</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1687,31 +1696,31 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E37">
         <v>187.142</v>
       </c>
       <c r="F37">
-        <v>30.69919240140126</v>
+        <v>60.27176651267052</v>
       </c>
       <c r="G37">
-        <v>280.6494709597861</v>
+        <v>230.4909888203641</v>
       </c>
       <c r="H37">
-        <v>2613.609135545783</v>
+        <v>954.4382874842486</v>
       </c>
       <c r="I37">
-        <v>89.14721586180441</v>
+        <v>140.302504619747</v>
       </c>
       <c r="J37">
-        <v>378.4536643616719</v>
+        <v>338.3488022024765</v>
       </c>
       <c r="K37">
-        <v>2585.021326445263</v>
+        <v>1427.77063818584</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1722,31 +1731,31 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E38">
         <v>188.142</v>
       </c>
       <c r="F38">
-        <v>30.16557147477723</v>
+        <v>59.22410781614111</v>
       </c>
       <c r="G38">
-        <v>293.4387630988585</v>
+        <v>240.9945418160856</v>
       </c>
       <c r="H38">
-        <v>2628.518389999867</v>
+        <v>959.8828518972249</v>
       </c>
       <c r="I38">
-        <v>142.9012207974494</v>
+        <v>224.9021351623825</v>
       </c>
       <c r="J38">
-        <v>316.4997005057176</v>
+        <v>282.9601207433769</v>
       </c>
       <c r="K38">
-        <v>2223.61285228014</v>
+        <v>1228.155879682441</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1757,31 +1766,31 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E39">
         <v>189.142</v>
       </c>
       <c r="F39">
-        <v>29.65883359760705</v>
+        <v>58.22922864744566</v>
       </c>
       <c r="G39">
-        <v>306.228055237931</v>
+        <v>251.498094811807</v>
       </c>
       <c r="H39">
-        <v>2642.923183471726</v>
+        <v>965.1431971515564</v>
       </c>
       <c r="I39">
-        <v>197.9788686518562</v>
+        <v>311.5849537768966</v>
       </c>
       <c r="J39">
-        <v>254.5457366497631</v>
+        <v>227.571439284277</v>
       </c>
       <c r="K39">
-        <v>1838.022921095609</v>
+        <v>1015.185109773</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1792,31 +1801,31 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E40">
         <v>190.142</v>
       </c>
       <c r="F40">
-        <v>29.17679556227887</v>
+        <v>57.28284271208796</v>
       </c>
       <c r="G40">
-        <v>319.0173473770033</v>
+        <v>262.0016478075285</v>
       </c>
       <c r="H40">
-        <v>2656.856538965278</v>
+        <v>970.2313825941735</v>
       </c>
       <c r="I40">
-        <v>254.4127529141714</v>
+        <v>400.402257053063</v>
       </c>
       <c r="J40">
-        <v>192.5917727938086</v>
+        <v>172.1827578251772</v>
       </c>
       <c r="K40">
-        <v>1428.251532891676</v>
+        <v>788.8583284575209</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1827,31 +1836,31 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E41">
         <v>191.142</v>
       </c>
       <c r="F41">
-        <v>28.7175145045943</v>
+        <v>56.38113558212471</v>
       </c>
       <c r="G41">
-        <v>331.8066395160757</v>
+        <v>272.5052008032499</v>
       </c>
       <c r="H41">
-        <v>2670.348339366529</v>
+        <v>975.1583208631431</v>
       </c>
       <c r="I41">
-        <v>312.2362696582238</v>
+        <v>491.4066047119828</v>
       </c>
       <c r="J41">
-        <v>130.6378089378544</v>
+        <v>116.7940763660776</v>
       </c>
       <c r="K41">
-        <v>994.2986876683399</v>
+        <v>549.1755357360025</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1862,31 +1871,31 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E42">
         <v>192.142</v>
       </c>
       <c r="F42">
-        <v>28.27925493161862</v>
+        <v>55.52069996189885</v>
       </c>
       <c r="G42">
-        <v>344.595931655148</v>
+        <v>283.0087537989714</v>
       </c>
       <c r="H42">
-        <v>2683.425713362727</v>
+        <v>979.9339188176995</v>
       </c>
       <c r="I42">
-        <v>371.4836373054397</v>
+        <v>584.6518507095409</v>
       </c>
       <c r="J42">
-        <v>68.68384508189989</v>
+        <v>61.40539490697778</v>
       </c>
       <c r="K42">
-        <v>536.164385425598</v>
+        <v>296.1367316084441</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1897,31 +1906,31 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E43">
         <v>193.142</v>
       </c>
       <c r="F43">
-        <v>27.86046111316957</v>
+        <v>54.69848148421151</v>
       </c>
       <c r="G43">
-        <v>357.3852237942205</v>
+        <v>293.5123067946928</v>
       </c>
       <c r="H43">
-        <v>2696.113363837922</v>
+        <v>984.5671974617975</v>
       </c>
       <c r="I43">
-        <v>432.189916874389</v>
+        <v>680.1931751057347</v>
       </c>
       <c r="J43">
-        <v>6.729881225945374</v>
+        <v>6.01671344787793</v>
       </c>
       <c r="K43">
-        <v>53.84862616345218</v>
+        <v>29.7419160748463</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1932,31 +1941,31 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E44">
         <v>194.142</v>
       </c>
       <c r="F44">
-        <v>27.4597338356582</v>
+        <v>53.91173307110599</v>
       </c>
       <c r="G44">
-        <v>370.1745159332929</v>
+        <v>304.0158597904143</v>
       </c>
       <c r="H44">
-        <v>2708.433848736853</v>
+        <v>989.0663945100415</v>
       </c>
       <c r="I44">
-        <v>494.3910327289701</v>
+        <v>778.0871167187772</v>
       </c>
       <c r="J44">
-        <v>-55.22408263000884</v>
+        <v>-49.37196801122165</v>
       </c>
       <c r="K44">
-        <v>-452.6485901180963</v>
+        <v>-250.0089108647901</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -1967,31 +1976,31 @@
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E45">
         <v>195.142</v>
       </c>
       <c r="F45">
-        <v>27.07581072660344</v>
+        <v>53.15797630496021</v>
       </c>
       <c r="G45">
-        <v>382.9638080723652</v>
+        <v>314.5194127861357</v>
       </c>
       <c r="H45">
-        <v>2720.407822421069</v>
+        <v>993.4390525261599</v>
       </c>
       <c r="I45">
-        <v>558.1237938374933</v>
+        <v>878.3916065832665</v>
       </c>
       <c r="J45">
-        <v>-117.1780464859633</v>
+        <v>-104.7606494703215</v>
       </c>
       <c r="K45">
-        <v>-983.3272634190505</v>
+        <v>-543.1157492104668</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2002,31 +2011,31 @@
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E46">
         <v>196.142</v>
       </c>
       <c r="F46">
-        <v>26.70754951937977</v>
+        <v>52.43496857214291</v>
       </c>
       <c r="G46">
-        <v>395.7531002114376</v>
+        <v>325.0229657818572</v>
       </c>
       <c r="H46">
-        <v>2732.054244004044</v>
+        <v>997.6920950028627</v>
       </c>
       <c r="I46">
-        <v>623.4259155552492</v>
+        <v>981.166002232231</v>
       </c>
       <c r="J46">
-        <v>-179.1320103419179</v>
+        <v>-160.1493309294214</v>
       </c>
       <c r="K46">
-        <v>-1538.18739373941</v>
+        <v>-849.5785989621836</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2037,31 +2046,31 @@
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E47">
         <v>197.142</v>
       </c>
       <c r="F47">
-        <v>26.35391375277303</v>
+        <v>51.74067498693194</v>
       </c>
       <c r="G47">
-        <v>408.54239235051</v>
+        <v>335.5265187775787</v>
       </c>
       <c r="H47">
-        <v>2743.390557942509</v>
+        <v>1001.831892310218</v>
       </c>
       <c r="I47">
-        <v>690.3360419434542</v>
+        <v>1086.471122823341</v>
       </c>
       <c r="J47">
-        <v>-241.0859741978724</v>
+        <v>-215.5380123885212</v>
       </c>
       <c r="K47">
-        <v>-2117.228981079173</v>
+        <v>-1169.397460119939</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2072,31 +2081,31 @@
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E48">
         <v>198.142</v>
       </c>
       <c r="F48">
-        <v>26.01396049756458</v>
+        <v>51.07324429510008</v>
       </c>
       <c r="G48">
-        <v>421.3316844895824</v>
+        <v>346.0300717733001</v>
       </c>
       <c r="H48">
-        <v>2754.432851202753</v>
+        <v>1005.864319089674</v>
       </c>
       <c r="I48">
-        <v>758.8937686377809</v>
+        <v>1194.369285130071</v>
       </c>
       <c r="J48">
-        <v>-303.0399380538263</v>
+        <v>-270.9266938476205</v>
       </c>
       <c r="K48">
-        <v>-2720.452025438336</v>
+        <v>-1502.572332683732</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2107,31 +2116,31 @@
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E49">
         <v>199.142</v>
       </c>
       <c r="F49">
-        <v>25.68682977917323</v>
+        <v>50.43098810737361</v>
       </c>
       <c r="G49">
-        <v>434.1209766286548</v>
+        <v>356.5336247690216</v>
       </c>
       <c r="H49">
-        <v>2765.195990556127</v>
+        <v>1009.794804391656</v>
       </c>
       <c r="I49">
-        <v>829.1396662800042</v>
+        <v>1304.924340419117</v>
       </c>
       <c r="J49">
-        <v>-364.9939019097808</v>
+        <v>-326.3153753067203</v>
       </c>
       <c r="K49">
-        <v>-3347.856526816906</v>
+        <v>-1849.103216653567</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2142,31 +2151,31 @@
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E50">
         <v>200.142</v>
       </c>
       <c r="F50">
-        <v>25.37173542619929</v>
+        <v>49.81236293236609</v>
       </c>
       <c r="G50">
-        <v>446.9102687677272</v>
+        <v>367.037177764743</v>
       </c>
       <c r="H50">
-        <v>2775.693742944294</v>
+        <v>1013.628375630572</v>
       </c>
       <c r="I50">
-        <v>901.1153045266259</v>
+        <v>1418.20171223587</v>
       </c>
       <c r="J50">
-        <v>-426.9478657657353</v>
+        <v>-381.7040567658202</v>
       </c>
       <c r="K50">
-        <v>-3999.442485214882</v>
+        <v>-2208.990112029441</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2177,31 +2186,31 @@
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E51">
         <v>201.142</v>
       </c>
       <c r="F51">
-        <v>25.06795712317097</v>
+        <v>49.21595457372464</v>
       </c>
       <c r="G51">
-        <v>459.6995609067995</v>
+        <v>377.5407307604645</v>
       </c>
       <c r="H51">
-        <v>2785.93888135931</v>
+        <v>1017.369697250121</v>
       </c>
       <c r="I51">
-        <v>974.8632766486976</v>
+        <v>1534.268435120338</v>
       </c>
       <c r="J51">
-        <v>-488.9018296216898</v>
+        <v>-437.09273822492</v>
       </c>
       <c r="K51">
-        <v>-4675.209900632262</v>
+        <v>-2582.233018811355</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2212,31 +2221,31 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E52">
         <v>202.142</v>
       </c>
       <c r="F52">
-        <v>24.7748334846327</v>
+        <v>48.64046453247792</v>
       </c>
       <c r="G52">
-        <v>472.488853045872</v>
+        <v>388.044283756186</v>
       </c>
       <c r="H52">
-        <v>2795.943278281288</v>
+        <v>1021.023104844876</v>
       </c>
       <c r="I52">
-        <v>1050.427224737386</v>
+        <v>1653.19319427641</v>
       </c>
       <c r="J52">
-        <v>-550.8557934776444</v>
+        <v>-492.4814196840199</v>
       </c>
       <c r="K52">
-        <v>-5375.158773069045</v>
+        <v>-2968.831936999307</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2247,31 +2256,31 @@
         <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E53">
         <v>203.142</v>
       </c>
       <c r="F53">
-        <v>24.49175599901589</v>
+        <v>48.08469811702943</v>
       </c>
       <c r="G53">
-        <v>485.2781451849443</v>
+        <v>398.5478367519074</v>
       </c>
       <c r="H53">
-        <v>2805.717988388031</v>
+        <v>1024.592635364208</v>
       </c>
       <c r="I53">
-        <v>1127.851865530199</v>
+        <v>1775.046366217926</v>
       </c>
       <c r="J53">
-        <v>-612.8097573335983</v>
+        <v>-547.8701011431192</v>
       </c>
       <c r="K53">
-        <v>-6099.289102525227</v>
+        <v>-3368.786866593297</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2282,31 +2291,1886 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E54">
         <v>204.142</v>
       </c>
       <c r="F54">
-        <v>24.21816371610231</v>
+        <v>47.54755401304697</v>
       </c>
       <c r="G54">
-        <v>498.0674373240167</v>
+        <v>409.0513897476288</v>
       </c>
       <c r="H54">
-        <v>2815.273321981598</v>
+        <v>1028.082053926207</v>
       </c>
       <c r="I54">
-        <v>1207.183016873172</v>
+        <v>1899.900060415642</v>
       </c>
       <c r="J54">
-        <v>-674.7637211895528</v>
+        <v>-603.2587826022191</v>
       </c>
       <c r="K54">
-        <v>-6847.60088900082</v>
+        <v>-3782.097807593329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55">
+        <v>708</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55">
+        <v>152.142</v>
+      </c>
+      <c r="F55">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G55">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H55">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I55">
+        <v>-959.2333485497459</v>
+      </c>
+      <c r="J55">
+        <v>1378.399518157884</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56">
+        <v>708</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56">
+        <v>153.142</v>
+      </c>
+      <c r="F56">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G56">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H56">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I56">
+        <v>-940.2955280629413</v>
+      </c>
+      <c r="J56">
+        <v>1344.868855267311</v>
+      </c>
+      <c r="K56">
+        <v>110.4127678046178</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57">
+        <v>708</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <v>154.142</v>
+      </c>
+      <c r="F57">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G57">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H57">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I57">
+        <v>-920.8913811691249</v>
+      </c>
+      <c r="J57">
+        <v>1311.338192376739</v>
+      </c>
+      <c r="K57">
+        <v>215.3198488925392</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58">
+        <v>708</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58">
+        <v>155.142</v>
+      </c>
+      <c r="F58">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G58">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H58">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I58">
+        <v>-901.0094250095358</v>
+      </c>
+      <c r="J58">
+        <v>1277.807529486166</v>
+      </c>
+      <c r="K58">
+        <v>314.7212432637649</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59">
+        <v>708</v>
+      </c>
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59">
+        <v>156.142</v>
+      </c>
+      <c r="F59">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G59">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H59">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I59">
+        <v>-880.6378939705812</v>
+      </c>
+      <c r="J59">
+        <v>1244.276866595593</v>
+      </c>
+      <c r="K59">
+        <v>408.6169509182943</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60">
+        <v>708</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60">
+        <v>157.142</v>
+      </c>
+      <c r="F60">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G60">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H60">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I60">
+        <v>-859.764732721257</v>
+      </c>
+      <c r="J60">
+        <v>1210.746203705021</v>
+      </c>
+      <c r="K60">
+        <v>497.0069718561281</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61">
+        <v>708</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61">
+        <v>158.142</v>
+      </c>
+      <c r="F61">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G61">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H61">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I61">
+        <v>-838.3775890791245</v>
+      </c>
+      <c r="J61">
+        <v>1177.215540814448</v>
+      </c>
+      <c r="K61">
+        <v>579.8913060772658</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62">
+        <v>708</v>
+      </c>
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62">
+        <v>159.142</v>
+      </c>
+      <c r="F62">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G62">
+        <v>-102.6982837471397</v>
+      </c>
+      <c r="H62">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I62">
+        <v>-816.4638067006159</v>
+      </c>
+      <c r="J62">
+        <v>1143.684877923876</v>
+      </c>
+      <c r="K62">
+        <v>657.2699535817075</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63">
+        <v>708</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63">
+        <v>160.142</v>
+      </c>
+      <c r="F63">
+        <v>240.5732305623948</v>
+      </c>
+      <c r="G63">
+        <v>-85.73990633398144</v>
+      </c>
+      <c r="H63">
+        <v>738.5042918601926</v>
+      </c>
+      <c r="I63">
+        <v>-794.0104175913468</v>
+      </c>
+      <c r="J63">
+        <v>1110.154215033303</v>
+      </c>
+      <c r="K63">
+        <v>729.1429143694529</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64">
+        <v>708</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64">
+        <v>161.142</v>
+      </c>
+      <c r="F64">
+        <v>186.7128913375429</v>
+      </c>
+      <c r="G64">
+        <v>-68.78152892082322</v>
+      </c>
+      <c r="H64">
+        <v>909.8323181351569</v>
+      </c>
+      <c r="I64">
+        <v>-771.004134432001</v>
+      </c>
+      <c r="J64">
+        <v>1076.623552142731</v>
+      </c>
+      <c r="K64">
+        <v>795.5101884405022</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65">
+        <v>708</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65">
+        <v>162.142</v>
+      </c>
+      <c r="F65">
+        <v>155.0726439692259</v>
+      </c>
+      <c r="G65">
+        <v>-51.82315150766501</v>
+      </c>
+      <c r="H65">
+        <v>1011.884052632433</v>
+      </c>
+      <c r="I65">
+        <v>-747.4313427152489</v>
+      </c>
+      <c r="J65">
+        <v>1043.092889252158</v>
+      </c>
+      <c r="K65">
+        <v>856.3717757948559</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66">
+        <v>708</v>
+      </c>
+      <c r="B66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66">
+        <v>163.142</v>
+      </c>
+      <c r="F66">
+        <v>135.0989985843533</v>
+      </c>
+      <c r="G66">
+        <v>-34.86477409450679</v>
+      </c>
+      <c r="H66">
+        <v>1084.813529864585</v>
+      </c>
+      <c r="I66">
+        <v>-723.278092689042</v>
+      </c>
+      <c r="J66">
+        <v>1009.562226361585</v>
+      </c>
+      <c r="K66">
+        <v>911.7276764325137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67">
+        <v>708</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67">
+        <v>164.142</v>
+      </c>
+      <c r="F67">
+        <v>121.1694593707297</v>
+      </c>
+      <c r="G67">
+        <v>-17.90639668134857</v>
+      </c>
+      <c r="H67">
+        <v>1141.603674713266</v>
+      </c>
+      <c r="I67">
+        <v>-698.5300911015225</v>
+      </c>
+      <c r="J67">
+        <v>976.0315634710126</v>
+      </c>
+      <c r="K67">
+        <v>961.5778903534754</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68">
+        <v>708</v>
+      </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68">
+        <v>165.142</v>
+      </c>
+      <c r="F68">
+        <v>110.7776059752617</v>
+      </c>
+      <c r="G68">
+        <v>-0.9480192681903654</v>
+      </c>
+      <c r="H68">
+        <v>1188.119208389497</v>
+      </c>
+      <c r="I68">
+        <v>-673.1726927426546</v>
+      </c>
+      <c r="J68">
+        <v>942.5009005804402</v>
+      </c>
+      <c r="K68">
+        <v>1005.922417557741</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69">
+        <v>708</v>
+      </c>
+      <c r="B69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69">
+        <v>166.142</v>
+      </c>
+      <c r="F69">
+        <v>102.6526277993096</v>
+      </c>
+      <c r="G69">
+        <v>16.01035814496785</v>
+      </c>
+      <c r="H69">
+        <v>1227.514469943877</v>
+      </c>
+      <c r="I69">
+        <v>-647.1908917775781</v>
+      </c>
+      <c r="J69">
+        <v>908.9702376898675</v>
+      </c>
+      <c r="K69">
+        <v>1044.76125804531</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70">
+        <v>708</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70">
+        <v>167.142</v>
+      </c>
+      <c r="F70">
+        <v>96.07892885590482</v>
+      </c>
+      <c r="G70">
+        <v>32.96873555812607</v>
+      </c>
+      <c r="H70">
+        <v>1261.682684395894</v>
+      </c>
+      <c r="I70">
+        <v>-620.5693128665552</v>
+      </c>
+      <c r="J70">
+        <v>875.4395747992951</v>
+      </c>
+      <c r="K70">
+        <v>1078.094411816184</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71">
+        <v>708</v>
+      </c>
+      <c r="B71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71">
+        <v>168.142</v>
+      </c>
+      <c r="F71">
+        <v>90.62041639272476</v>
+      </c>
+      <c r="G71">
+        <v>49.92711297128428</v>
+      </c>
+      <c r="H71">
+        <v>1291.849836685835</v>
+      </c>
+      <c r="I71">
+        <v>-593.292202066252</v>
+      </c>
+      <c r="J71">
+        <v>841.9089119087224</v>
+      </c>
+      <c r="K71">
+        <v>1105.921878870362</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72">
+        <v>708</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72">
+        <v>169.142</v>
+      </c>
+      <c r="F72">
+        <v>85.99473778221251</v>
+      </c>
+      <c r="G72">
+        <v>66.88549038444251</v>
+      </c>
+      <c r="H72">
+        <v>1318.855508487563</v>
+      </c>
+      <c r="I72">
+        <v>-565.343417506973</v>
+      </c>
+      <c r="J72">
+        <v>808.3782490181499</v>
+      </c>
+      <c r="K72">
+        <v>1128.243659207843</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>708</v>
+      </c>
+      <c r="B73" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73">
+        <v>170.142</v>
+      </c>
+      <c r="F73">
+        <v>82.01016694215582</v>
+      </c>
+      <c r="G73">
+        <v>83.84386779760072</v>
+      </c>
+      <c r="H73">
+        <v>1343.299930576936</v>
+      </c>
+      <c r="I73">
+        <v>-536.7064198403319</v>
+      </c>
+      <c r="J73">
+        <v>774.8475861275774</v>
+      </c>
+      <c r="K73">
+        <v>1145.059752828628</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74">
+        <v>708</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74">
+        <v>171.142</v>
+      </c>
+      <c r="F74">
+        <v>78.53143070910021</v>
+      </c>
+      <c r="G74">
+        <v>100.8022452107589</v>
+      </c>
+      <c r="H74">
+        <v>1365.627119038931</v>
+      </c>
+      <c r="I74">
+        <v>-507.3642624517047</v>
+      </c>
+      <c r="J74">
+        <v>741.3169232370047</v>
+      </c>
+      <c r="K74">
+        <v>1156.370159732718</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75">
+        <v>708</v>
+      </c>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75">
+        <v>172.142</v>
+      </c>
+      <c r="F75">
+        <v>75.46003540670539</v>
+      </c>
+      <c r="G75">
+        <v>117.7606226239172</v>
+      </c>
+      <c r="H75">
+        <v>1386.174782334632</v>
+      </c>
+      <c r="I75">
+        <v>-477.2995814316723</v>
+      </c>
+      <c r="J75">
+        <v>707.7862603464323</v>
+      </c>
+      <c r="K75">
+        <v>1162.174879920112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76">
+        <v>708</v>
+      </c>
+      <c r="B76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76">
+        <v>173.142</v>
+      </c>
+      <c r="F76">
+        <v>72.72235665239742</v>
+      </c>
+      <c r="G76">
+        <v>134.7190000370753</v>
+      </c>
+      <c r="H76">
+        <v>1405.205763915588</v>
+      </c>
+      <c r="I76">
+        <v>-446.4945853005209</v>
+      </c>
+      <c r="J76">
+        <v>674.2555974558596</v>
+      </c>
+      <c r="K76">
+        <v>1162.473913390809</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>708</v>
+      </c>
+      <c r="B77" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77">
+        <v>174.142</v>
+      </c>
+      <c r="F77">
+        <v>70.26211993278559</v>
+      </c>
+      <c r="G77">
+        <v>151.6773774502336</v>
+      </c>
+      <c r="H77">
+        <v>1422.928656256441</v>
+      </c>
+      <c r="I77">
+        <v>-414.9310444797169</v>
+      </c>
+      <c r="J77">
+        <v>640.724934565287</v>
+      </c>
+      <c r="K77">
+        <v>1157.267260144811</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78">
+        <v>708</v>
+      </c>
+      <c r="B78" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78">
+        <v>175.142</v>
+      </c>
+      <c r="F78">
+        <v>68.03548161964743</v>
+      </c>
+      <c r="G78">
+        <v>168.6357548633918</v>
+      </c>
+      <c r="H78">
+        <v>1439.511774488562</v>
+      </c>
+      <c r="I78">
+        <v>-382.5902805041253</v>
+      </c>
+      <c r="J78">
+        <v>607.1942716747145</v>
+      </c>
+      <c r="K78">
+        <v>1146.554920182116</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79">
+        <v>708</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79">
+        <v>176.142</v>
+      </c>
+      <c r="F79">
+        <v>66.00771167430617</v>
+      </c>
+      <c r="G79">
+        <v>185.59413227655</v>
+      </c>
+      <c r="H79">
+        <v>1455.092901883778</v>
+      </c>
+      <c r="I79">
+        <v>-349.4531549685922</v>
+      </c>
+      <c r="J79">
+        <v>573.6636087841418</v>
+      </c>
+      <c r="K79">
+        <v>1130.336893502726</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80">
+        <v>708</v>
+      </c>
+      <c r="B80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80">
+        <v>177.142</v>
+      </c>
+      <c r="F80">
+        <v>64.15089673946457</v>
+      </c>
+      <c r="G80">
+        <v>202.5525096897082</v>
+      </c>
+      <c r="H80">
+        <v>1469.786255199646</v>
+      </c>
+      <c r="I80">
+        <v>-315.5000582023433</v>
+      </c>
+      <c r="J80">
+        <v>540.1329458935693</v>
+      </c>
+      <c r="K80">
+        <v>1108.613180106639</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81">
+        <v>708</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81">
+        <v>178.142</v>
+      </c>
+      <c r="F81">
+        <v>62.44231265172765</v>
+      </c>
+      <c r="G81">
+        <v>219.5108871028664</v>
+      </c>
+      <c r="H81">
+        <v>1483.687570456594</v>
+      </c>
+      <c r="I81">
+        <v>-280.7108976645018</v>
+      </c>
+      <c r="J81">
+        <v>506.6022830029968</v>
+      </c>
+      <c r="K81">
+        <v>1081.383779993857</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82">
+        <v>708</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82">
+        <v>179.142</v>
+      </c>
+      <c r="F82">
+        <v>60.86324758421846</v>
+      </c>
+      <c r="G82">
+        <v>236.4692645160247</v>
+      </c>
+      <c r="H82">
+        <v>1496.877886738695</v>
+      </c>
+      <c r="I82">
+        <v>-245.0650860538564</v>
+      </c>
+      <c r="J82">
+        <v>473.0716201124241</v>
+      </c>
+      <c r="K82">
+        <v>1048.648693164378</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83">
+        <v>708</v>
+      </c>
+      <c r="B83" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83">
+        <v>180.142</v>
+      </c>
+      <c r="F83">
+        <v>59.39813552923872</v>
+      </c>
+      <c r="G83">
+        <v>253.4276419291828</v>
+      </c>
+      <c r="H83">
+        <v>1509.426408583862</v>
+      </c>
+      <c r="I83">
+        <v>-208.5415291258444</v>
+      </c>
+      <c r="J83">
+        <v>439.5409572218515</v>
+      </c>
+      <c r="K83">
+        <v>1010.407919618203</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84">
+        <v>708</v>
+      </c>
+      <c r="B84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84">
+        <v>181.142</v>
+      </c>
+      <c r="F84">
+        <v>58.03390788941457</v>
+      </c>
+      <c r="G84">
+        <v>270.3860193423411</v>
+      </c>
+      <c r="H84">
+        <v>1521.392703757215</v>
+      </c>
+      <c r="I84">
+        <v>-171.1186132095364</v>
+      </c>
+      <c r="J84">
+        <v>406.0102943312791</v>
+      </c>
+      <c r="K84">
+        <v>966.6614593553331</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85">
+        <v>708</v>
+      </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85">
+        <v>182.142</v>
+      </c>
+      <c r="F85">
+        <v>56.75950117227188</v>
+      </c>
+      <c r="G85">
+        <v>287.3443967554993</v>
+      </c>
+      <c r="H85">
+        <v>1532.828413399164</v>
+      </c>
+      <c r="I85">
+        <v>-132.7741924172407</v>
+      </c>
+      <c r="J85">
+        <v>372.4796314407064</v>
+      </c>
+      <c r="K85">
+        <v>917.4093123757664</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86">
+        <v>708</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" t="s">
+        <v>14</v>
+      </c>
+      <c r="D86" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86">
+        <v>183.142</v>
+      </c>
+      <c r="F86">
+        <v>55.56547825912346</v>
+      </c>
+      <c r="G86">
+        <v>304.3027741686575</v>
+      </c>
+      <c r="H86">
+        <v>1543.778598879229</v>
+      </c>
+      <c r="I86">
+        <v>-93.48557553915478</v>
+      </c>
+      <c r="J86">
+        <v>338.9489685501339</v>
+      </c>
+      <c r="K86">
+        <v>862.6514786795041</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87">
+        <v>708</v>
+      </c>
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87">
+        <v>184.142</v>
+      </c>
+      <c r="F87">
+        <v>54.4437335441293</v>
+      </c>
+      <c r="G87">
+        <v>321.2611515818157</v>
+      </c>
+      <c r="H87">
+        <v>1554.282814204856</v>
+      </c>
+      <c r="I87">
+        <v>-53.22951261531069</v>
+      </c>
+      <c r="J87">
+        <v>305.4183056595613</v>
+      </c>
+      <c r="K87">
+        <v>802.3879582665454</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88">
+        <v>708</v>
+      </c>
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88">
+        <v>185.142</v>
+      </c>
+      <c r="F88">
+        <v>53.38726085267539</v>
+      </c>
+      <c r="G88">
+        <v>338.219528994974</v>
+      </c>
+      <c r="H88">
+        <v>1564.375968473238</v>
+      </c>
+      <c r="I88">
+        <v>-11.98218117686593</v>
+      </c>
+      <c r="J88">
+        <v>271.8876427689887</v>
+      </c>
+      <c r="K88">
+        <v>736.6187511368908</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89">
+        <v>708</v>
+      </c>
+      <c r="B89" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89">
+        <v>186.142</v>
+      </c>
+      <c r="F89">
+        <v>52.38996893743865</v>
+      </c>
+      <c r="G89">
+        <v>355.1779064081322</v>
+      </c>
+      <c r="H89">
+        <v>1574.089025839693</v>
+      </c>
+      <c r="I89">
+        <v>30.28082785140153</v>
+      </c>
+      <c r="J89">
+        <v>238.3569798784162</v>
+      </c>
+      <c r="K89">
+        <v>665.3438572905403</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90">
+        <v>708</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" t="s">
+        <v>16</v>
+      </c>
+      <c r="E90">
+        <v>187.142</v>
+      </c>
+      <c r="F90">
+        <v>51.44653344364868</v>
+      </c>
+      <c r="G90">
+        <v>372.1362838212904</v>
+      </c>
+      <c r="H90">
+        <v>1583.449578406337</v>
+      </c>
+      <c r="I90">
+        <v>73.58452459573466</v>
+      </c>
+      <c r="J90">
+        <v>204.8263169878435</v>
+      </c>
+      <c r="K90">
+        <v>588.5632767274939</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91">
+        <v>708</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" t="s">
+        <v>16</v>
+      </c>
+      <c r="E91">
+        <v>188.142</v>
+      </c>
+      <c r="F91">
+        <v>50.5522771228687</v>
+      </c>
+      <c r="G91">
+        <v>389.0946612344486</v>
+      </c>
+      <c r="H91">
+        <v>1592.482318749411</v>
+      </c>
+      <c r="I91">
+        <v>117.9545350337269</v>
+      </c>
+      <c r="J91">
+        <v>171.2956540972711</v>
+      </c>
+      <c r="K91">
+        <v>506.2770094477515</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92">
+        <v>708</v>
+      </c>
+      <c r="B92" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" t="s">
+        <v>16</v>
+      </c>
+      <c r="E92">
+        <v>189.142</v>
+      </c>
+      <c r="F92">
+        <v>49.70307214040117</v>
+      </c>
+      <c r="G92">
+        <v>406.0530386476069</v>
+      </c>
+      <c r="H92">
+        <v>1601.209432471135</v>
+      </c>
+      <c r="I92">
+        <v>163.4171161590931</v>
+      </c>
+      <c r="J92">
+        <v>137.7649912066985</v>
+      </c>
+      <c r="K92">
+        <v>418.4850554513126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93">
+        <v>708</v>
+      </c>
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" t="s">
+        <v>16</v>
+      </c>
+      <c r="E93">
+        <v>190.142</v>
+      </c>
+      <c r="F93">
+        <v>48.89525981813012</v>
+      </c>
+      <c r="G93">
+        <v>423.011416060765</v>
+      </c>
+      <c r="H93">
+        <v>1609.650926488734</v>
+      </c>
+      <c r="I93">
+        <v>209.9991715198641</v>
+      </c>
+      <c r="J93">
+        <v>104.2343283161258</v>
+      </c>
+      <c r="K93">
+        <v>325.1874147381781</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94">
+        <v>708</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94">
+        <v>191.142</v>
+      </c>
+      <c r="F94">
+        <v>48.12558425190496</v>
+      </c>
+      <c r="G94">
+        <v>439.9697934739232</v>
+      </c>
+      <c r="H94">
+        <v>1617.824905285622</v>
+      </c>
+      <c r="I94">
+        <v>257.7282671391883</v>
+      </c>
+      <c r="J94">
+        <v>70.70366542555334</v>
+      </c>
+      <c r="K94">
+        <v>226.3840873083477</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95">
+        <v>708</v>
+      </c>
+      <c r="B95" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95">
+        <v>192.142</v>
+      </c>
+      <c r="F95">
+        <v>47.39113705592389</v>
+      </c>
+      <c r="G95">
+        <v>456.9281708870814</v>
+      </c>
+      <c r="H95">
+        <v>1625.747804719709</v>
+      </c>
+      <c r="I95">
+        <v>306.6326478281765</v>
+      </c>
+      <c r="J95">
+        <v>37.1730025349807</v>
+      </c>
+      <c r="K95">
+        <v>122.0750731618209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96">
+        <v>708</v>
+      </c>
+      <c r="B96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96">
+        <v>193.142</v>
+      </c>
+      <c r="F96">
+        <v>46.68931109564721</v>
+      </c>
+      <c r="G96">
+        <v>473.8865483002397</v>
+      </c>
+      <c r="H96">
+        <v>1633.43459098116</v>
+      </c>
+      <c r="I96">
+        <v>356.7412539004254</v>
+      </c>
+      <c r="J96">
+        <v>3.642339644408074</v>
+      </c>
+      <c r="K96">
+        <v>12.26037229859828</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97">
+        <v>708</v>
+      </c>
+      <c r="B97" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" t="s">
+        <v>16</v>
+      </c>
+      <c r="E97">
+        <v>194.142</v>
+      </c>
+      <c r="F97">
+        <v>46.01776153125768</v>
+      </c>
+      <c r="G97">
+        <v>490.8449257133979</v>
+      </c>
+      <c r="H97">
+        <v>1640.898930753181</v>
+      </c>
+      <c r="I97">
+        <v>408.0837382981308</v>
+      </c>
+      <c r="J97">
+        <v>-29.8883232461644</v>
+      </c>
+      <c r="K97">
+        <v>-103.0600152813201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98">
+        <v>708</v>
+      </c>
+      <c r="B98" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98">
+        <v>195.142</v>
+      </c>
+      <c r="F98">
+        <v>45.37437284495224</v>
+      </c>
+      <c r="G98">
+        <v>507.803303126556</v>
+      </c>
+      <c r="H98">
+        <v>1648.153337437125</v>
+      </c>
+      <c r="I98">
+        <v>460.6904841399103</v>
+      </c>
+      <c r="J98">
+        <v>-63.41898613673703</v>
+      </c>
+      <c r="K98">
+        <v>-223.8860895779347</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99">
+        <v>708</v>
+      </c>
+      <c r="B99" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" t="s">
+        <v>16</v>
+      </c>
+      <c r="E99">
+        <v>196.142</v>
+      </c>
+      <c r="F99">
+        <v>44.75723079555533</v>
+      </c>
+      <c r="G99">
+        <v>524.7616805397143</v>
+      </c>
+      <c r="H99">
+        <v>1655.209297371875</v>
+      </c>
+      <c r="I99">
+        <v>514.5926227007253</v>
+      </c>
+      <c r="J99">
+        <v>-96.94964902730966</v>
+      </c>
+      <c r="K99">
+        <v>-350.2178505912457</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100">
+        <v>708</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E100">
+        <v>197.142</v>
+      </c>
+      <c r="F100">
+        <v>44.16459845344937</v>
+      </c>
+      <c r="G100">
+        <v>541.7200579528725</v>
+      </c>
+      <c r="H100">
+        <v>1662.077379244719</v>
+      </c>
+      <c r="I100">
+        <v>569.8220518345421</v>
+      </c>
+      <c r="J100">
+        <v>-130.4803119178823</v>
+      </c>
+      <c r="K100">
+        <v>-482.0552983212525</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101">
+        <v>708</v>
+      </c>
+      <c r="B101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" t="s">
+        <v>16</v>
+      </c>
+      <c r="E101">
+        <v>198.142</v>
+      </c>
+      <c r="F101">
+        <v>43.59489563245396</v>
+      </c>
+      <c r="G101">
+        <v>558.6784353660307</v>
+      </c>
+      <c r="H101">
+        <v>1668.767329310233</v>
+      </c>
+      <c r="I101">
+        <v>626.4114548506356</v>
+      </c>
+      <c r="J101">
+        <v>-164.0109748084546</v>
+      </c>
+      <c r="K101">
+        <v>-619.3984327679542</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102">
+        <v>708</v>
+      </c>
+      <c r="B102" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E102">
+        <v>199.142</v>
+      </c>
+      <c r="F102">
+        <v>43.04668116400439</v>
+      </c>
+      <c r="G102">
+        <v>575.636812779189</v>
+      </c>
+      <c r="H102">
+        <v>1675.288154570461</v>
+      </c>
+      <c r="I102">
+        <v>684.394319854705</v>
+      </c>
+      <c r="J102">
+        <v>-197.5416376990273</v>
+      </c>
+      <c r="K102">
+        <v>-762.2472539313529</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103">
+        <v>708</v>
+      </c>
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" t="s">
+        <v>16</v>
+      </c>
+      <c r="E103">
+        <v>200.142</v>
+      </c>
+      <c r="F103">
+        <v>42.51863756089519</v>
+      </c>
+      <c r="G103">
+        <v>592.5951901923472</v>
+      </c>
+      <c r="H103">
+        <v>1681.648195697952</v>
+      </c>
+      <c r="I103">
+        <v>743.8049595662415</v>
+      </c>
+      <c r="J103">
+        <v>-231.0723005895999</v>
+      </c>
+      <c r="K103">
+        <v>-910.6017618114478</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104">
+        <v>708</v>
+      </c>
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" t="s">
+        <v>16</v>
+      </c>
+      <c r="E104">
+        <v>201.142</v>
+      </c>
+      <c r="F104">
+        <v>42.00955769905858</v>
+      </c>
+      <c r="G104">
+        <v>609.5535676055054</v>
+      </c>
+      <c r="H104">
+        <v>1687.855191182984</v>
+      </c>
+      <c r="I104">
+        <v>804.6785316238881</v>
+      </c>
+      <c r="J104">
+        <v>-264.6029634801725</v>
+      </c>
+      <c r="K104">
+        <v>-1064.461956408239</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105">
+        <v>708</v>
+      </c>
+      <c r="B105" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E105">
+        <v>202.142</v>
+      </c>
+      <c r="F105">
+        <v>41.51833321093506</v>
+      </c>
+      <c r="G105">
+        <v>626.5119450186636</v>
+      </c>
+      <c r="H105">
+        <v>1693.916333942576</v>
+      </c>
+      <c r="I105">
+        <v>867.0510593907958</v>
+      </c>
+      <c r="J105">
+        <v>-298.1336263707452</v>
+      </c>
+      <c r="K105">
+        <v>-1223.827837721725</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106">
+        <v>708</v>
+      </c>
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" t="s">
+        <v>16</v>
+      </c>
+      <c r="E106">
+        <v>203.142</v>
+      </c>
+      <c r="F106">
+        <v>41.04394433644909</v>
+      </c>
+      <c r="G106">
+        <v>643.4703224318218</v>
+      </c>
+      <c r="H106">
+        <v>1699.838321429941</v>
+      </c>
+      <c r="I106">
+        <v>930.9594532722886</v>
+      </c>
+      <c r="J106">
+        <v>-331.6642892613175</v>
+      </c>
+      <c r="K106">
+        <v>-1388.699405751907</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107">
+        <v>708</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" t="s">
+        <v>16</v>
+      </c>
+      <c r="E107">
+        <v>204.142</v>
+      </c>
+      <c r="F107">
+        <v>40.58545102011692</v>
+      </c>
+      <c r="G107">
+        <v>660.42869984498</v>
+      </c>
+      <c r="H107">
+        <v>1705.627400119822</v>
+      </c>
+      <c r="I107">
+        <v>996.4415325584699</v>
+      </c>
+      <c r="J107">
+        <v>-365.1949521518901</v>
+      </c>
+      <c r="K107">
+        <v>-1559.076660498786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds preliminary asset support for graphing
</commit_message>
<xml_diff>
--- a/runs/run708/NotionalETEOutput708.xlsx
+++ b/runs/run708/NotionalETEOutput708.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="17">
   <si>
     <t>uniqueid</t>
   </si>
@@ -52,10 +52,19 @@
     <t>Missile_SOMERSAULT_State_Update</t>
   </si>
   <si>
-    <t>MISSILE_SOMERSAULT_93.MISSILE_SOMERSAULT_93</t>
+    <t>Missile_HELLMASKER_State_Update</t>
+  </si>
+  <si>
+    <t>MISSILE_SOMERSAULT_39.MISSILE_SOMERSAULT_39</t>
+  </si>
+  <si>
+    <t>MISSILE_HELLMASKER_298.MISSILE_HELLMASKER_298</t>
   </si>
   <si>
     <t>MISSILE_SOMERSAULT</t>
+  </si>
+  <si>
+    <t>MISSILE_HELLMASKER</t>
   </si>
 </sst>
 </file>
@@ -413,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,31 +471,31 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>152.142</v>
       </c>
       <c r="F2">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G2">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H2">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I2">
-        <v>1114861.266385574</v>
+        <v>1114860.769705735</v>
       </c>
       <c r="J2">
-        <v>4843221.686686004</v>
+        <v>4843216.49510044</v>
       </c>
       <c r="K2">
-        <v>3984374.524075927</v>
+        <v>3984366.387583164</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -497,31 +506,31 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>153.142</v>
       </c>
       <c r="F3">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G3">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H3">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I3">
-        <v>1114890.880379619</v>
+        <v>1114890.383686587</v>
       </c>
       <c r="J3">
-        <v>4843173.03511372</v>
+        <v>4843167.843580307</v>
       </c>
       <c r="K3">
-        <v>3984678.320388361</v>
+        <v>3984670.183275216</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -532,31 +541,31 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>154.142</v>
       </c>
       <c r="F4">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G4">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H4">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I4">
-        <v>1114921.223591024</v>
+        <v>1114920.726884474</v>
       </c>
       <c r="J4">
-        <v>4843124.383541435</v>
+        <v>4843119.192060173</v>
       </c>
       <c r="K4">
-        <v>3984966.968024106</v>
+        <v>3984958.830321514</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -567,31 +576,31 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>155.142</v>
       </c>
       <c r="F5">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G5">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H5">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I5">
-        <v>1114952.313976094</v>
+        <v>1114951.817255693</v>
       </c>
       <c r="J5">
-        <v>4843075.731969152</v>
+        <v>4843070.54054004</v>
       </c>
       <c r="K5">
-        <v>3985240.46698316</v>
+        <v>3985232.328722055</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -602,31 +611,31 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>156.142</v>
       </c>
       <c r="F6">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G6">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H6">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I6">
-        <v>1114984.169933294</v>
+        <v>1114983.6731987</v>
       </c>
       <c r="J6">
-        <v>4843027.080396867</v>
+        <v>4843021.889019907</v>
       </c>
       <c r="K6">
-        <v>3985498.817265524</v>
+        <v>3985490.678476842</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -637,31 +646,31 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>157.142</v>
       </c>
       <c r="F7">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G7">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H7">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I7">
-        <v>1115016.810314133</v>
+        <v>1115016.313564998</v>
       </c>
       <c r="J7">
-        <v>4842978.428824584</v>
+        <v>4842973.237499774</v>
       </c>
       <c r="K7">
-        <v>3985742.018871198</v>
+        <v>3985733.879585874</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -672,31 +681,31 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>158.142</v>
       </c>
       <c r="F8">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G8">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H8">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I8">
-        <v>1115050.254434321</v>
+        <v>1115049.757670287</v>
       </c>
       <c r="J8">
-        <v>4842929.777252299</v>
+        <v>4842924.58597964</v>
       </c>
       <c r="K8">
-        <v>3985970.071800181</v>
+        <v>3985961.93204915</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -707,31 +716,31 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>159.142</v>
       </c>
       <c r="F9">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G9">
-        <v>4841130.472756287</v>
+        <v>4841132.743961312</v>
       </c>
       <c r="H9">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I9">
-        <v>1115084.522085201</v>
+        <v>1115084.0253059</v>
       </c>
       <c r="J9">
-        <v>4842881.125680014</v>
+        <v>4842875.934459507</v>
       </c>
       <c r="K9">
-        <v>3986182.976052474</v>
+        <v>3986174.835866671</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -742,31 +751,31 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>160.142</v>
       </c>
       <c r="F10">
-        <v>1116578.600334327</v>
+        <v>1116579.191078848</v>
       </c>
       <c r="G10">
-        <v>4841146.985595655</v>
+        <v>4841149.256808426</v>
       </c>
       <c r="H10">
-        <v>3985229.595963211</v>
+        <v>3985227.019403234</v>
       </c>
       <c r="I10">
-        <v>1115119.633545459</v>
+        <v>1115119.136750515</v>
       </c>
       <c r="J10">
-        <v>4842832.474107731</v>
+        <v>4842827.282939374</v>
       </c>
       <c r="K10">
-        <v>3986380.731628077</v>
+        <v>3986372.591038437</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -777,31 +786,31 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>161.142</v>
       </c>
       <c r="F11">
-        <v>1116529.91976635</v>
+        <v>1116530.510485117</v>
       </c>
       <c r="G11">
-        <v>4841163.498435021</v>
+        <v>4841165.769655541</v>
       </c>
       <c r="H11">
-        <v>3985428.850433365</v>
+        <v>3985426.273744564</v>
       </c>
       <c r="I11">
-        <v>1115155.609593123</v>
+        <v>1115155.112782152</v>
       </c>
       <c r="J11">
-        <v>4842783.822535447</v>
+        <v>4842778.631419241</v>
       </c>
       <c r="K11">
-        <v>3986563.338526989</v>
+        <v>3986555.197564448</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -812,31 +821,31 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>162.142</v>
       </c>
       <c r="F12">
-        <v>1116501.322374745</v>
+        <v>1116501.913078382</v>
       </c>
       <c r="G12">
-        <v>4841180.011274389</v>
+        <v>4841182.282502655</v>
       </c>
       <c r="H12">
-        <v>3985547.536586048</v>
+        <v>3985544.959820513</v>
       </c>
       <c r="I12">
-        <v>1115192.471517864</v>
+        <v>1115191.97469047</v>
       </c>
       <c r="J12">
-        <v>4842735.170963163</v>
+        <v>4842729.979899107</v>
       </c>
       <c r="K12">
-        <v>3986730.796749211</v>
+        <v>3986722.655444704</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -847,31 +856,31 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <v>163.142</v>
       </c>
       <c r="F13">
-        <v>1116483.269603153</v>
+        <v>1116483.860297238</v>
       </c>
       <c r="G13">
-        <v>4841196.524113757</v>
+        <v>4841198.795349769</v>
       </c>
       <c r="H13">
-        <v>3985632.35355768</v>
+        <v>3985629.776737309</v>
       </c>
       <c r="I13">
-        <v>1115230.241133589</v>
+        <v>1115229.744289369</v>
       </c>
       <c r="J13">
-        <v>4842686.519390878</v>
+        <v>4842681.328378974</v>
       </c>
       <c r="K13">
-        <v>3986883.106294743</v>
+        <v>3986874.964679203</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -882,31 +891,31 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <v>164.142</v>
       </c>
       <c r="F14">
-        <v>1116470.679673526</v>
+        <v>1116471.27036095</v>
       </c>
       <c r="G14">
-        <v>4841213.036953123</v>
+        <v>4841215.308196883</v>
       </c>
       <c r="H14">
-        <v>3985698.400488049</v>
+        <v>3985695.823624977</v>
       </c>
       <c r="I14">
-        <v>1115268.940791353</v>
+        <v>1115268.443929892</v>
       </c>
       <c r="J14">
-        <v>4842637.867818595</v>
+        <v>4842632.676858841</v>
       </c>
       <c r="K14">
-        <v>3987020.267163584</v>
+        <v>3987012.125267949</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -917,31 +926,31 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <v>165.142</v>
       </c>
       <c r="F15">
-        <v>1116461.287208998</v>
+        <v>1116461.877891453</v>
       </c>
       <c r="G15">
-        <v>4841229.549792491</v>
+        <v>4841231.821043998</v>
       </c>
       <c r="H15">
-        <v>3985752.498047089</v>
+        <v>3985749.921149041</v>
       </c>
       <c r="I15">
-        <v>1115308.593392588</v>
+        <v>1115308.096513461</v>
       </c>
       <c r="J15">
-        <v>4842589.216246311</v>
+        <v>4842584.025338708</v>
       </c>
       <c r="K15">
-        <v>3987142.279355736</v>
+        <v>3987134.137210939</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -952,31 +961,31 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <v>166.142</v>
       </c>
       <c r="F16">
-        <v>1116453.943613356</v>
+        <v>1116454.534291926</v>
       </c>
       <c r="G16">
-        <v>4841246.062631858</v>
+        <v>4841248.333891111</v>
       </c>
       <c r="H16">
-        <v>3985798.314730665</v>
+        <v>3985795.737802995</v>
       </c>
       <c r="I16">
-        <v>1115349.222402648</v>
+        <v>1115348.725505421</v>
       </c>
       <c r="J16">
-        <v>4842540.564674025</v>
+        <v>4842535.373818574</v>
       </c>
       <c r="K16">
-        <v>3987249.142871197</v>
+        <v>3987241.000508174</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -987,31 +996,31 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>167.142</v>
       </c>
       <c r="F17">
-        <v>1116448.002109777</v>
+        <v>1116448.592785204</v>
       </c>
       <c r="G17">
-        <v>4841262.575471225</v>
+        <v>4841264.846738226</v>
       </c>
       <c r="H17">
-        <v>3985838.052359206</v>
+        <v>3985835.475405844</v>
       </c>
       <c r="I17">
-        <v>1115390.851864703</v>
+        <v>1115390.354948929</v>
       </c>
       <c r="J17">
-        <v>4842491.913101742</v>
+        <v>4842486.722298442</v>
       </c>
       <c r="K17">
-        <v>3987340.857709967</v>
+        <v>3987332.715159653</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1022,31 +1031,31 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>168.142</v>
       </c>
       <c r="F18">
-        <v>1116443.06854473</v>
+        <v>1116443.659217546</v>
       </c>
       <c r="G18">
-        <v>4841279.088310593</v>
+        <v>4841281.359585341</v>
       </c>
       <c r="H18">
-        <v>3985873.136753021</v>
+        <v>3985870.559776977</v>
       </c>
       <c r="I18">
-        <v>1115433.506413962</v>
+        <v>1115433.009479185</v>
       </c>
       <c r="J18">
-        <v>4842443.261529458</v>
+        <v>4842438.070778309</v>
       </c>
       <c r="K18">
-        <v>3987417.423872047</v>
+        <v>3987409.281165378</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1057,31 +1066,31 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>169.142</v>
       </c>
       <c r="F19">
-        <v>1116438.887719557</v>
+        <v>1116439.478390162</v>
       </c>
       <c r="G19">
-        <v>4841295.601149959</v>
+        <v>4841297.872432454</v>
       </c>
       <c r="H19">
-        <v>3985904.54434548</v>
+        <v>3985901.96734913</v>
       </c>
       <c r="I19">
-        <v>1115477.211292255</v>
+        <v>1115476.714338008</v>
       </c>
       <c r="J19">
-        <v>4842394.609957174</v>
+        <v>4842389.419258176</v>
       </c>
       <c r="K19">
-        <v>3987478.841357437</v>
+        <v>3987470.698525347</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1092,31 +1101,31 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E20">
         <v>170.142</v>
       </c>
       <c r="F20">
-        <v>1116435.286346554</v>
+        <v>1116435.877015253</v>
       </c>
       <c r="G20">
-        <v>4841312.113989327</v>
+        <v>4841314.385279569</v>
       </c>
       <c r="H20">
-        <v>3985932.973204888</v>
+        <v>3985930.396190158</v>
       </c>
       <c r="I20">
-        <v>1115521.992362969</v>
+        <v>1115521.495388771</v>
       </c>
       <c r="J20">
-        <v>4842345.958384889</v>
+        <v>4842340.767738042</v>
       </c>
       <c r="K20">
-        <v>3987525.110166137</v>
+        <v>3987516.967239561</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1127,31 +1136,31 @@
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E21">
         <v>171.142</v>
       </c>
       <c r="F21">
-        <v>1116432.142161833</v>
+        <v>1116432.732828869</v>
       </c>
       <c r="G21">
-        <v>4841328.626828695</v>
+        <v>4841330.898126683</v>
       </c>
       <c r="H21">
-        <v>3985958.939721889</v>
+        <v>3985956.362690371</v>
       </c>
       <c r="I21">
-        <v>1115567.876126351</v>
+        <v>1115567.379131712</v>
       </c>
       <c r="J21">
-        <v>4842297.306812605</v>
+        <v>4842292.116217909</v>
       </c>
       <c r="K21">
-        <v>3987556.230298147</v>
+        <v>3987548.08730802</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1162,31 +1171,31 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E22">
         <v>172.142</v>
       </c>
       <c r="F22">
-        <v>1116429.366143896</v>
+        <v>1116429.956809463</v>
       </c>
       <c r="G22">
-        <v>4841345.139668061</v>
+        <v>4841347.410973798</v>
       </c>
       <c r="H22">
-        <v>3985982.836651375</v>
+        <v>3985980.259604407</v>
       </c>
       <c r="I22">
-        <v>1115614.889735194</v>
+        <v>1115614.39271961</v>
       </c>
       <c r="J22">
-        <v>4842248.655240322</v>
+        <v>4842243.464697776</v>
       </c>
       <c r="K22">
-        <v>3987572.201753465</v>
+        <v>3987564.058730724</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1197,31 +1206,31 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E23">
         <v>173.142</v>
       </c>
       <c r="F23">
-        <v>1116426.891748847</v>
+        <v>1116427.482413105</v>
       </c>
       <c r="G23">
-        <v>4841361.652507429</v>
+        <v>4841363.923820912</v>
       </c>
       <c r="H23">
-        <v>3986004.969680242</v>
+        <v>3986002.392618965</v>
       </c>
       <c r="I23">
-        <v>1115663.061010903</v>
+        <v>1115662.563973859</v>
       </c>
       <c r="J23">
-        <v>4842200.003668037</v>
+        <v>4842194.813177643</v>
       </c>
       <c r="K23">
-        <v>3987573.024532094</v>
+        <v>3987564.881507673</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1232,31 +1241,31 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>174.142</v>
       </c>
       <c r="F24">
-        <v>1116424.668114117</v>
+        <v>1116425.258777198</v>
       </c>
       <c r="G24">
-        <v>4841378.165346797</v>
+        <v>4841380.436668026</v>
       </c>
       <c r="H24">
-        <v>3986025.581401511</v>
+        <v>3986023.004326907</v>
       </c>
       <c r="I24">
-        <v>1115712.41845996</v>
+        <v>1115711.921400926</v>
       </c>
       <c r="J24">
-        <v>4842151.352095753</v>
+        <v>4842146.161657509</v>
       </c>
       <c r="K24">
-        <v>3987558.698634032</v>
+        <v>3987550.555638866</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1267,31 +1276,31 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E25">
         <v>175.142</v>
       </c>
       <c r="F25">
-        <v>1116422.655612538</v>
+        <v>1116423.246274554</v>
       </c>
       <c r="G25">
-        <v>4841394.678186163</v>
+        <v>4841396.94951514</v>
       </c>
       <c r="H25">
-        <v>3986044.867565652</v>
+        <v>3986042.29047858</v>
       </c>
       <c r="I25">
-        <v>1115762.991290792</v>
+        <v>1115762.494209227</v>
       </c>
       <c r="J25">
-        <v>4842102.700523469</v>
+        <v>4842097.510137377</v>
       </c>
       <c r="K25">
-        <v>3987529.22405928</v>
+        <v>3987521.081124304</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1302,31 +1311,31 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E26">
         <v>176.142</v>
       </c>
       <c r="F26">
-        <v>1116420.822854072</v>
+        <v>1116421.413515119</v>
       </c>
       <c r="G26">
-        <v>4841411.191025531</v>
+        <v>4841413.462362255</v>
       </c>
       <c r="H26">
-        <v>3986062.988414593</v>
+        <v>3986060.411315805</v>
       </c>
       <c r="I26">
-        <v>1115814.809431056</v>
+        <v>1115814.312326407</v>
       </c>
       <c r="J26">
-        <v>4842054.048951185</v>
+        <v>4842048.858617244</v>
       </c>
       <c r="K26">
-        <v>3987484.600807839</v>
+        <v>3987476.457963987</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1337,31 +1346,31 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E27">
         <v>177.142</v>
       </c>
       <c r="F27">
-        <v>1116419.144609803</v>
+        <v>1116419.735269962</v>
       </c>
       <c r="G27">
-        <v>4841427.703864898</v>
+        <v>4841429.975209368</v>
       </c>
       <c r="H27">
-        <v>3986080.076782406</v>
+        <v>3986077.49967257</v>
       </c>
       <c r="I27">
-        <v>1115867.903545354</v>
+        <v>1115867.40641705</v>
       </c>
       <c r="J27">
-        <v>4842005.3973789</v>
+        <v>4842000.20709711</v>
       </c>
       <c r="K27">
-        <v>3987424.828879706</v>
+        <v>3987416.686157915</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1372,31 +1381,31 @@
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E28">
         <v>178.142</v>
       </c>
       <c r="F28">
-        <v>1116417.600340958</v>
+        <v>1116418.1910003</v>
       </c>
       <c r="G28">
-        <v>4841444.216704265</v>
+        <v>4841446.488056483</v>
       </c>
       <c r="H28">
-        <v>3986096.24401007</v>
+        <v>3986093.666889781</v>
       </c>
       <c r="I28">
-        <v>1115922.30505337</v>
+        <v>1115921.807900829</v>
       </c>
       <c r="J28">
-        <v>4841956.745806616</v>
+        <v>4841951.555576977</v>
       </c>
       <c r="K28">
-        <v>3987349.908274883</v>
+        <v>3987341.765706087</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1407,31 +1416,31 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E29">
         <v>179.142</v>
       </c>
       <c r="F29">
-        <v>1116416.173135236</v>
+        <v>1116416.763793822</v>
       </c>
       <c r="G29">
-        <v>4841460.729543633</v>
+        <v>4841463.000903598</v>
       </c>
       <c r="H29">
-        <v>3986111.584346028</v>
+        <v>3986109.00721582</v>
       </c>
       <c r="I29">
-        <v>1115978.046148472</v>
+        <v>1115977.548971099</v>
       </c>
       <c r="J29">
-        <v>4841908.094234332</v>
+        <v>4841902.904056844</v>
       </c>
       <c r="K29">
-        <v>3987259.838993371</v>
+        <v>3987251.696608505</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1442,31 +1451,31 @@
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E30">
         <v>180.142</v>
       </c>
       <c r="F30">
-        <v>1116414.848923617</v>
+        <v>1116415.439581503</v>
       </c>
       <c r="G30">
-        <v>4841477.242383</v>
+        <v>4841479.513750711</v>
       </c>
       <c r="H30">
-        <v>3986126.178275146</v>
+        <v>3986123.601135504</v>
       </c>
       <c r="I30">
-        <v>1116035.15981676</v>
+        <v>1116034.662613943</v>
       </c>
       <c r="J30">
-        <v>4841859.442662048</v>
+        <v>4841854.252536711</v>
       </c>
       <c r="K30">
-        <v>3987154.621035167</v>
+        <v>3987146.478865168</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1477,31 +1486,31 @@
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E31">
         <v>181.142</v>
       </c>
       <c r="F31">
-        <v>1116413.615894317</v>
+        <v>1116414.206551551</v>
       </c>
       <c r="G31">
-        <v>4841493.755222368</v>
+        <v>4841496.026597826</v>
       </c>
       <c r="H31">
-        <v>3986140.095074728</v>
+        <v>3986137.517926088</v>
       </c>
       <c r="I31">
-        <v>1116093.679856587</v>
+        <v>1116093.182627698</v>
       </c>
       <c r="J31">
-        <v>4841810.791089764</v>
+        <v>4841805.601016577</v>
       </c>
       <c r="K31">
-        <v>3987034.254400273</v>
+        <v>3987026.112476075</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1512,31 +1521,31 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <v>182.142</v>
       </c>
       <c r="F32">
-        <v>1116412.464047825</v>
+        <v>1116413.054704449</v>
       </c>
       <c r="G32">
-        <v>4841510.268061736</v>
+        <v>4841512.53944494</v>
       </c>
       <c r="H32">
-        <v>3986153.394803413</v>
+        <v>3986150.817646174</v>
       </c>
       <c r="I32">
-        <v>1116153.640898556</v>
+        <v>1116153.143642954</v>
       </c>
       <c r="J32">
-        <v>4841762.13951748</v>
+        <v>4841756.949496444</v>
       </c>
       <c r="K32">
-        <v>3986898.739088689</v>
+        <v>3986890.597441227</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1547,31 +1556,31 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E33">
         <v>183.142</v>
       </c>
       <c r="F33">
-        <v>1116411.384854592</v>
+        <v>1116411.975510646</v>
       </c>
       <c r="G33">
-        <v>4841526.780901102</v>
+        <v>4841529.052292055</v>
       </c>
       <c r="H33">
-        <v>3986166.129867566</v>
+        <v>3986163.552702094</v>
       </c>
       <c r="I33">
-        <v>1116215.078426021</v>
+        <v>1116214.581143048</v>
       </c>
       <c r="J33">
-        <v>4841713.487945196</v>
+        <v>4841708.297976312</v>
       </c>
       <c r="K33">
-        <v>3986748.075100415</v>
+        <v>3986739.933760623</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1582,31 +1591,31 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E34">
         <v>184.142</v>
       </c>
       <c r="F34">
-        <v>1116410.370988534</v>
+        <v>1116410.961644051</v>
       </c>
       <c r="G34">
-        <v>4841543.29374047</v>
+        <v>4841545.565139169</v>
       </c>
       <c r="H34">
-        <v>3986178.346268493</v>
+        <v>3986175.769095123</v>
       </c>
       <c r="I34">
-        <v>1116278.028796079</v>
+        <v>1116277.531485061</v>
       </c>
       <c r="J34">
-        <v>4841664.836372912</v>
+        <v>4841659.646456179</v>
       </c>
       <c r="K34">
-        <v>3986582.262435451</v>
+        <v>3986574.121434265</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1617,31 +1626,31 @@
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E35">
         <v>185.142</v>
       </c>
       <c r="F35">
-        <v>1116409.416117261</v>
+        <v>1116410.006772273</v>
       </c>
       <c r="G35">
-        <v>4841559.806579837</v>
+        <v>4841562.077986282</v>
       </c>
       <c r="H35">
-        <v>3986190.08460547</v>
+        <v>3986187.50742451</v>
       </c>
       <c r="I35">
-        <v>1116342.529261085</v>
+        <v>1116342.031921332</v>
       </c>
       <c r="J35">
-        <v>4841616.184800627</v>
+        <v>4841610.994936045</v>
       </c>
       <c r="K35">
-        <v>3986401.301093796</v>
+        <v>3986393.160462151</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1652,31 +1661,31 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E36">
         <v>186.142</v>
       </c>
       <c r="F36">
-        <v>1116408.514735324</v>
+        <v>1116409.105389859</v>
       </c>
       <c r="G36">
-        <v>4841576.319419204</v>
+        <v>4841578.590833398</v>
       </c>
       <c r="H36">
-        <v>3986201.380889803</v>
+        <v>3986198.80370154</v>
       </c>
       <c r="I36">
-        <v>1116408.617990703</v>
+        <v>1116408.120621507</v>
       </c>
       <c r="J36">
-        <v>4841567.533228343</v>
+        <v>4841562.343415912</v>
       </c>
       <c r="K36">
-        <v>3986205.191075451</v>
+        <v>3986197.050844282</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1687,31 +1696,31 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E37">
         <v>187.142</v>
       </c>
       <c r="F37">
-        <v>1116407.662030415</v>
+        <v>1116408.252684498</v>
       </c>
       <c r="G37">
-        <v>4841592.832258572</v>
+        <v>4841595.103680512</v>
       </c>
       <c r="H37">
-        <v>3986212.267211105</v>
+        <v>3986209.690015804</v>
       </c>
       <c r="I37">
-        <v>1116476.334094488</v>
+        <v>1116475.836695123</v>
       </c>
       <c r="J37">
-        <v>4841518.881656059</v>
+        <v>4841513.691895779</v>
       </c>
       <c r="K37">
-        <v>3985993.932380415</v>
+        <v>3985985.792580659</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1722,31 +1731,31 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E38">
         <v>188.142</v>
       </c>
       <c r="F38">
-        <v>1116406.853775097</v>
+        <v>1116407.444428753</v>
       </c>
       <c r="G38">
-        <v>4841609.345097939</v>
+        <v>4841611.616527625</v>
       </c>
       <c r="H38">
-        <v>3986222.772286837</v>
+        <v>3986220.195084744</v>
       </c>
       <c r="I38">
-        <v>1116545.71764503</v>
+        <v>1116545.220214755</v>
       </c>
       <c r="J38">
-        <v>4841470.230083776</v>
+        <v>4841465.040375646</v>
       </c>
       <c r="K38">
-        <v>3985767.52500869</v>
+        <v>3985759.385671279</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1757,31 +1766,31 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E39">
         <v>189.142</v>
       </c>
       <c r="F39">
-        <v>1116406.086238511</v>
+        <v>1116406.676891761</v>
       </c>
       <c r="G39">
-        <v>4841625.857937306</v>
+        <v>4841628.12937474</v>
       </c>
       <c r="H39">
-        <v>3986232.921918852</v>
+        <v>3986230.344710197</v>
       </c>
       <c r="I39">
-        <v>1116616.809701673</v>
+        <v>1116616.312239726</v>
       </c>
       <c r="J39">
-        <v>4841421.57851149</v>
+        <v>4841416.388855512</v>
       </c>
       <c r="K39">
-        <v>3985525.968960273</v>
+        <v>3985517.830116145</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1792,31 +1801,31 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E40">
         <v>190.142</v>
       </c>
       <c r="F40">
-        <v>1116405.356113836</v>
+        <v>1116405.9467667</v>
       </c>
       <c r="G40">
-        <v>4841642.370776674</v>
+        <v>4841644.642221855</v>
       </c>
       <c r="H40">
-        <v>3986242.739375193</v>
+        <v>3986240.16216019</v>
       </c>
       <c r="I40">
-        <v>1116689.652334808</v>
+        <v>1116689.154840408</v>
       </c>
       <c r="J40">
-        <v>4841372.926939206</v>
+        <v>4841367.737335379</v>
       </c>
       <c r="K40">
-        <v>3985269.264235167</v>
+        <v>3985261.125915255</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1827,31 +1836,31 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E41">
         <v>191.142</v>
       </c>
       <c r="F41">
-        <v>1116404.66045829</v>
+        <v>1116405.251110785</v>
       </c>
       <c r="G41">
-        <v>4841658.88361604</v>
+        <v>4841661.155068968</v>
       </c>
       <c r="H41">
-        <v>3986252.245711369</v>
+        <v>3986249.66849022</v>
       </c>
       <c r="I41">
-        <v>1116764.288650769</v>
+        <v>1116763.791123118</v>
       </c>
       <c r="J41">
-        <v>4841324.275366923</v>
+        <v>4841319.085815246</v>
       </c>
       <c r="K41">
-        <v>3984997.41083337</v>
+        <v>3984989.273068611</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1862,31 +1871,31 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E42">
         <v>192.142</v>
       </c>
       <c r="F42">
-        <v>1116403.996643186</v>
+        <v>1116404.587295331</v>
       </c>
       <c r="G42">
-        <v>4841675.396455408</v>
+        <v>4841677.667916083</v>
       </c>
       <c r="H42">
-        <v>3986261.460042282</v>
+        <v>3986258.882815177</v>
       </c>
       <c r="I42">
-        <v>1116840.762817346</v>
+        <v>1116840.265255626</v>
       </c>
       <c r="J42">
-        <v>4841275.623794639</v>
+        <v>4841270.434295114</v>
       </c>
       <c r="K42">
-        <v>3984710.408754883</v>
+        <v>3984702.27157621</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1897,31 +1906,31 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E43">
         <v>193.142</v>
       </c>
       <c r="F43">
-        <v>1116403.362312121</v>
+        <v>1116403.95296393</v>
       </c>
       <c r="G43">
-        <v>4841691.909294776</v>
+        <v>4841694.180763197</v>
       </c>
       <c r="H43">
-        <v>3986270.399773609</v>
+        <v>3986267.822540724</v>
       </c>
       <c r="I43">
-        <v>1116919.120089921</v>
+        <v>1116918.622493292</v>
       </c>
       <c r="J43">
-        <v>4841226.972222354</v>
+        <v>4841221.78277498</v>
       </c>
       <c r="K43">
-        <v>3984408.257999706</v>
+        <v>3984400.121438056</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1932,31 +1941,31 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E44">
         <v>194.142</v>
       </c>
       <c r="F44">
-        <v>1116402.755345757</v>
+        <v>1116403.345997245</v>
       </c>
       <c r="G44">
-        <v>4841708.422134142</v>
+        <v>4841710.693610311</v>
       </c>
       <c r="H44">
-        <v>3986279.080799701</v>
+        <v>3986276.503561203</v>
       </c>
       <c r="I44">
-        <v>1116999.406838245</v>
+        <v>1116998.909205847</v>
       </c>
       <c r="J44">
-        <v>4841178.32065007</v>
+        <v>4841173.131254847</v>
       </c>
       <c r="K44">
-        <v>3984090.958567839</v>
+        <v>3984082.822654145</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -1967,31 +1976,31 @@
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E45">
         <v>195.142</v>
       </c>
       <c r="F45">
-        <v>1116402.173832029</v>
+        <v>1116402.764483209</v>
       </c>
       <c r="G45">
-        <v>4841724.93497351</v>
+        <v>4841727.206457426</v>
       </c>
       <c r="H45">
-        <v>3986287.517673641</v>
+        <v>3986284.940429688</v>
       </c>
       <c r="I45">
-        <v>1117081.670573885</v>
+        <v>1117081.172904838</v>
       </c>
       <c r="J45">
-        <v>4841129.669077787</v>
+        <v>4841124.479734714</v>
       </c>
       <c r="K45">
-        <v>3983758.510459281</v>
+        <v>3983750.37522448</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2002,31 +2011,31 @@
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E46">
         <v>196.142</v>
       </c>
       <c r="F46">
-        <v>1116401.616040787</v>
+        <v>1116402.206691673</v>
       </c>
       <c r="G46">
-        <v>4841741.447812877</v>
+        <v>4841743.719304539</v>
       </c>
       <c r="H46">
-        <v>3986295.72375404</v>
+        <v>3986293.146504782</v>
       </c>
       <c r="I46">
-        <v>1117165.959978333</v>
+        <v>1117165.462271735</v>
       </c>
       <c r="J46">
-        <v>4841081.017505501</v>
+        <v>4841075.82821458</v>
       </c>
       <c r="K46">
-        <v>3983410.913674032</v>
+        <v>3983402.779149059</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2037,31 +2046,31 @@
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E47">
         <v>197.142</v>
       </c>
       <c r="F47">
-        <v>1116401.080402144</v>
+        <v>1116401.671052746</v>
       </c>
       <c r="G47">
-        <v>4841757.960652244</v>
+        <v>4841760.232151655</v>
       </c>
       <c r="H47">
-        <v>3986303.71133228</v>
+        <v>3986301.134077858</v>
       </c>
       <c r="I47">
-        <v>1117252.324931821</v>
+        <v>1117251.827186746</v>
       </c>
       <c r="J47">
-        <v>4841032.365933217</v>
+        <v>4841027.176694447</v>
       </c>
       <c r="K47">
-        <v>3983048.168212094</v>
+        <v>3983040.034427884</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2072,31 +2081,31 @@
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E48">
         <v>198.142</v>
       </c>
       <c r="F48">
-        <v>1116400.565487881</v>
+        <v>1116401.15613821</v>
       </c>
       <c r="G48">
-        <v>4841774.473491612</v>
+        <v>4841776.744998769</v>
       </c>
       <c r="H48">
-        <v>3986311.491743253</v>
+        <v>3986308.9144838</v>
       </c>
       <c r="I48">
-        <v>1117340.816542835</v>
+        <v>1117340.318758336</v>
       </c>
       <c r="J48">
-        <v>4840983.714360934</v>
+        <v>4840978.525174314</v>
       </c>
       <c r="K48">
-        <v>3982670.274073465</v>
+        <v>3982662.141060952</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2107,31 +2116,31 @@
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E49">
         <v>199.142</v>
       </c>
       <c r="F49">
-        <v>1116400.069995426</v>
+        <v>1116400.660645493</v>
       </c>
       <c r="G49">
-        <v>4841790.986330979</v>
+        <v>4841793.257845882</v>
       </c>
       <c r="H49">
-        <v>3986319.075462101</v>
+        <v>3986316.498197746</v>
       </c>
       <c r="I49">
-        <v>1117431.487178358</v>
+        <v>1117430.989353465</v>
       </c>
       <c r="J49">
-        <v>4840935.062788649</v>
+        <v>4840929.873654181</v>
       </c>
       <c r="K49">
-        <v>3982277.231258146</v>
+        <v>3982269.099048266</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2142,31 +2151,31 @@
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E50">
         <v>200.142</v>
       </c>
       <c r="F50">
-        <v>1116399.592733996</v>
+        <v>1116400.183383811</v>
       </c>
       <c r="G50">
-        <v>4841807.499170346</v>
+        <v>4841809.770692997</v>
       </c>
       <c r="H50">
-        <v>3986326.472189027</v>
+        <v>3986323.89491989</v>
       </c>
       <c r="I50">
-        <v>1117524.390494866</v>
+        <v>1117523.892628584</v>
       </c>
       <c r="J50">
-        <v>4840886.411216365</v>
+        <v>4840881.222134048</v>
       </c>
       <c r="K50">
-        <v>3981869.039766137</v>
+        <v>3981860.908389825</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2177,31 +2186,31 @@
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E51">
         <v>201.142</v>
       </c>
       <c r="F51">
-        <v>1116399.132612557</v>
+        <v>1116399.723262128</v>
       </c>
       <c r="G51">
-        <v>4841824.012009714</v>
+        <v>4841826.283540112</v>
       </c>
       <c r="H51">
-        <v>3986333.690923892</v>
+        <v>3986331.113650087</v>
       </c>
       <c r="I51">
-        <v>1117619.581470074</v>
+        <v>1117619.083561383</v>
       </c>
       <c r="J51">
-        <v>4840837.759644081</v>
+        <v>4840832.570613915</v>
       </c>
       <c r="K51">
-        <v>3981445.699597437</v>
+        <v>3981437.569085628</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2212,31 +2221,31 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E52">
         <v>202.142</v>
       </c>
       <c r="F52">
-        <v>1116398.688629332</v>
+        <v>1116399.279278668</v>
       </c>
       <c r="G52">
-        <v>4841840.52484908</v>
+        <v>4841842.796387225</v>
       </c>
       <c r="H52">
-        <v>3986340.740032058</v>
+        <v>3986338.162753696</v>
       </c>
       <c r="I52">
-        <v>1117717.116435472</v>
+        <v>1117716.618483328</v>
       </c>
       <c r="J52">
-        <v>4840789.108071798</v>
+        <v>4840783.919093782</v>
       </c>
       <c r="K52">
-        <v>3981007.210752047</v>
+        <v>3980999.081135676</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2247,31 +2256,31 @@
         <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E53">
         <v>203.142</v>
       </c>
       <c r="F53">
-        <v>1116398.259862633</v>
+        <v>1116398.850511743</v>
       </c>
       <c r="G53">
-        <v>4841857.037688448</v>
+        <v>4841859.30923434</v>
       </c>
       <c r="H53">
-        <v>3986347.627302662</v>
+        <v>3986345.050019847</v>
       </c>
       <c r="I53">
-        <v>1117817.053109662</v>
+        <v>1117816.555112996</v>
       </c>
       <c r="J53">
-        <v>4840740.456499513</v>
+        <v>4840735.267573649</v>
       </c>
       <c r="K53">
-        <v>3980553.573229967</v>
+        <v>3980545.44453997</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2282,31 +2291,1886 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E54">
         <v>204.142</v>
       </c>
       <c r="F54">
-        <v>1116397.84546281</v>
+        <v>1116398.4361117</v>
       </c>
       <c r="G54">
-        <v>4841873.550527817</v>
+        <v>4841875.822081455</v>
       </c>
       <c r="H54">
-        <v>3986354.360000354</v>
+        <v>3986351.782713186</v>
       </c>
       <c r="I54">
-        <v>1117919.450632514</v>
+        <v>1117918.95259023</v>
       </c>
       <c r="J54">
-        <v>4840691.804927228</v>
+        <v>4840686.616053515</v>
       </c>
       <c r="K54">
-        <v>3980084.787031197</v>
+        <v>3980076.659298507</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55">
+        <v>708</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55">
+        <v>152.142</v>
+      </c>
+      <c r="F55">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G55">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H55">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I55">
+        <v>1114862.740616727</v>
+      </c>
+      <c r="J55">
+        <v>4843222.935572709</v>
+      </c>
+      <c r="K55">
+        <v>3984374.863249617</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56">
+        <v>708</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56">
+        <v>153.142</v>
+      </c>
+      <c r="F56">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G56">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H56">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I56">
+        <v>1114892.354649932</v>
+      </c>
+      <c r="J56">
+        <v>4843174.28398788</v>
+      </c>
+      <c r="K56">
+        <v>3984678.659587913</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57">
+        <v>708</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <v>154.142</v>
+      </c>
+      <c r="F57">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G57">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H57">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I57">
+        <v>1114922.697901461</v>
+      </c>
+      <c r="J57">
+        <v>4843125.63240305</v>
+      </c>
+      <c r="K57">
+        <v>3984967.307248229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58">
+        <v>708</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58">
+        <v>155.142</v>
+      </c>
+      <c r="F58">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G58">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H58">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I58">
+        <v>1114953.788327643</v>
+      </c>
+      <c r="J58">
+        <v>4843076.98081822</v>
+      </c>
+      <c r="K58">
+        <v>3985240.806230565</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59">
+        <v>708</v>
+      </c>
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59">
+        <v>156.142</v>
+      </c>
+      <c r="F59">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G59">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H59">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I59">
+        <v>1114985.644326968</v>
+      </c>
+      <c r="J59">
+        <v>4843028.32923339</v>
+      </c>
+      <c r="K59">
+        <v>3985499.156534921</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60">
+        <v>708</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60">
+        <v>157.142</v>
+      </c>
+      <c r="F60">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G60">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H60">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I60">
+        <v>1115018.284750969</v>
+      </c>
+      <c r="J60">
+        <v>4842979.677648561</v>
+      </c>
+      <c r="K60">
+        <v>3985742.358161298</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61">
+        <v>708</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61">
+        <v>158.142</v>
+      </c>
+      <c r="F61">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G61">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H61">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I61">
+        <v>1115051.728915382</v>
+      </c>
+      <c r="J61">
+        <v>4842931.026063731</v>
+      </c>
+      <c r="K61">
+        <v>3985970.411109694</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62">
+        <v>708</v>
+      </c>
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62">
+        <v>159.142</v>
+      </c>
+      <c r="F62">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G62">
+        <v>4841118.549191112</v>
+      </c>
+      <c r="H62">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I62">
+        <v>1115085.996611576</v>
+      </c>
+      <c r="J62">
+        <v>4842882.374478902</v>
+      </c>
+      <c r="K62">
+        <v>3986183.31538011</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63">
+        <v>708</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63">
+        <v>160.142</v>
+      </c>
+      <c r="F63">
+        <v>1116578.821065525</v>
+      </c>
+      <c r="G63">
+        <v>4841135.061989809</v>
+      </c>
+      <c r="H63">
+        <v>3985228.479036027</v>
+      </c>
+      <c r="I63">
+        <v>1115121.108118262</v>
+      </c>
+      <c r="J63">
+        <v>4842833.722894073</v>
+      </c>
+      <c r="K63">
+        <v>3986381.070972547</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64">
+        <v>708</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64">
+        <v>161.142</v>
+      </c>
+      <c r="F64">
+        <v>1116530.140487925</v>
+      </c>
+      <c r="G64">
+        <v>4841151.574788505</v>
+      </c>
+      <c r="H64">
+        <v>3985427.733450336</v>
+      </c>
+      <c r="I64">
+        <v>1115157.084213499</v>
+      </c>
+      <c r="J64">
+        <v>4842785.071309243</v>
+      </c>
+      <c r="K64">
+        <v>3986563.677887004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65">
+        <v>708</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65">
+        <v>162.142</v>
+      </c>
+      <c r="F65">
+        <v>1116501.543090667</v>
+      </c>
+      <c r="G65">
+        <v>4841168.087587202</v>
+      </c>
+      <c r="H65">
+        <v>3985546.419569755</v>
+      </c>
+      <c r="I65">
+        <v>1115193.946186984</v>
+      </c>
+      <c r="J65">
+        <v>4842736.419724413</v>
+      </c>
+      <c r="K65">
+        <v>3986731.136123482</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66">
+        <v>708</v>
+      </c>
+      <c r="B66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66">
+        <v>163.142</v>
+      </c>
+      <c r="F66">
+        <v>1116483.490315506</v>
+      </c>
+      <c r="G66">
+        <v>4841184.6003859</v>
+      </c>
+      <c r="H66">
+        <v>3985631.236517617</v>
+      </c>
+      <c r="I66">
+        <v>1115231.715852654</v>
+      </c>
+      <c r="J66">
+        <v>4842687.768139583</v>
+      </c>
+      <c r="K66">
+        <v>3986883.445681978</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67">
+        <v>708</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67">
+        <v>164.142</v>
+      </c>
+      <c r="F67">
+        <v>1116470.90038339</v>
+      </c>
+      <c r="G67">
+        <v>4841201.113184595</v>
+      </c>
+      <c r="H67">
+        <v>3985697.283429475</v>
+      </c>
+      <c r="I67">
+        <v>1115270.415561593</v>
+      </c>
+      <c r="J67">
+        <v>4842639.116554754</v>
+      </c>
+      <c r="K67">
+        <v>3987020.606562496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68">
+        <v>708</v>
+      </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68">
+        <v>165.142</v>
+      </c>
+      <c r="F68">
+        <v>1116461.507917005</v>
+      </c>
+      <c r="G68">
+        <v>4841217.625983292</v>
+      </c>
+      <c r="H68">
+        <v>3985751.380973353</v>
+      </c>
+      <c r="I68">
+        <v>1115310.068215262</v>
+      </c>
+      <c r="J68">
+        <v>4842590.464969925</v>
+      </c>
+      <c r="K68">
+        <v>3987142.618765034</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69">
+        <v>708</v>
+      </c>
+      <c r="B69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69">
+        <v>166.142</v>
+      </c>
+      <c r="F69">
+        <v>1116454.164319912</v>
+      </c>
+      <c r="G69">
+        <v>4841234.138781988</v>
+      </c>
+      <c r="H69">
+        <v>3985797.197644088</v>
+      </c>
+      <c r="I69">
+        <v>1115350.697279047</v>
+      </c>
+      <c r="J69">
+        <v>4842541.813385095</v>
+      </c>
+      <c r="K69">
+        <v>3987249.482289592</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70">
+        <v>708</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70">
+        <v>167.142</v>
+      </c>
+      <c r="F70">
+        <v>1116448.222815158</v>
+      </c>
+      <c r="G70">
+        <v>4841250.651580686</v>
+      </c>
+      <c r="H70">
+        <v>3985836.935261491</v>
+      </c>
+      <c r="I70">
+        <v>1115392.326796151</v>
+      </c>
+      <c r="J70">
+        <v>4842493.161800265</v>
+      </c>
+      <c r="K70">
+        <v>3987341.197136169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71">
+        <v>708</v>
+      </c>
+      <c r="B71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71">
+        <v>168.142</v>
+      </c>
+      <c r="F71">
+        <v>1116443.289249136</v>
+      </c>
+      <c r="G71">
+        <v>4841267.164379383</v>
+      </c>
+      <c r="H71">
+        <v>3985872.019645474</v>
+      </c>
+      <c r="I71">
+        <v>1115434.981401814</v>
+      </c>
+      <c r="J71">
+        <v>4842444.510215436</v>
+      </c>
+      <c r="K71">
+        <v>3987417.763304767</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72">
+        <v>708</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72">
+        <v>169.142</v>
+      </c>
+      <c r="F72">
+        <v>1116439.108423137</v>
+      </c>
+      <c r="G72">
+        <v>4841283.677178078</v>
+      </c>
+      <c r="H72">
+        <v>3985903.42722913</v>
+      </c>
+      <c r="I72">
+        <v>1115478.6863379</v>
+      </c>
+      <c r="J72">
+        <v>4842395.858630607</v>
+      </c>
+      <c r="K72">
+        <v>3987479.180795386</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>708</v>
+      </c>
+      <c r="B73" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73">
+        <v>170.142</v>
+      </c>
+      <c r="F73">
+        <v>1116435.507049422</v>
+      </c>
+      <c r="G73">
+        <v>4841300.189976775</v>
+      </c>
+      <c r="H73">
+        <v>3985931.85608057</v>
+      </c>
+      <c r="I73">
+        <v>1115523.46746783</v>
+      </c>
+      <c r="J73">
+        <v>4842347.207045777</v>
+      </c>
+      <c r="K73">
+        <v>3987525.449608024</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74">
+        <v>708</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74">
+        <v>171.142</v>
+      </c>
+      <c r="F74">
+        <v>1116432.362864079</v>
+      </c>
+      <c r="G74">
+        <v>4841316.702775473</v>
+      </c>
+      <c r="H74">
+        <v>3985957.822590294</v>
+      </c>
+      <c r="I74">
+        <v>1115569.351291886</v>
+      </c>
+      <c r="J74">
+        <v>4842298.555460947</v>
+      </c>
+      <c r="K74">
+        <v>3987556.569742682</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75">
+        <v>708</v>
+      </c>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75">
+        <v>172.142</v>
+      </c>
+      <c r="F75">
+        <v>1116429.586845593</v>
+      </c>
+      <c r="G75">
+        <v>4841333.215574169</v>
+      </c>
+      <c r="H75">
+        <v>3985981.719513082</v>
+      </c>
+      <c r="I75">
+        <v>1115616.364962897</v>
+      </c>
+      <c r="J75">
+        <v>4842249.903876117</v>
+      </c>
+      <c r="K75">
+        <v>3987572.541199361</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76">
+        <v>708</v>
+      </c>
+      <c r="B76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76">
+        <v>173.142</v>
+      </c>
+      <c r="F76">
+        <v>1116427.112450055</v>
+      </c>
+      <c r="G76">
+        <v>4841349.728372865</v>
+      </c>
+      <c r="H76">
+        <v>3986003.852535747</v>
+      </c>
+      <c r="I76">
+        <v>1115664.536302306</v>
+      </c>
+      <c r="J76">
+        <v>4842201.252291288</v>
+      </c>
+      <c r="K76">
+        <v>3987573.36397806</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>708</v>
+      </c>
+      <c r="B77" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77">
+        <v>174.142</v>
+      </c>
+      <c r="F77">
+        <v>1116424.888814886</v>
+      </c>
+      <c r="G77">
+        <v>4841366.241171562</v>
+      </c>
+      <c r="H77">
+        <v>3986024.464251238</v>
+      </c>
+      <c r="I77">
+        <v>1115713.89381663</v>
+      </c>
+      <c r="J77">
+        <v>4842152.600706458</v>
+      </c>
+      <c r="K77">
+        <v>3987559.038078778</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78">
+        <v>708</v>
+      </c>
+      <c r="B78" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78">
+        <v>175.142</v>
+      </c>
+      <c r="F78">
+        <v>1116422.876312908</v>
+      </c>
+      <c r="G78">
+        <v>4841382.753970259</v>
+      </c>
+      <c r="H78">
+        <v>3986043.750409975</v>
+      </c>
+      <c r="I78">
+        <v>1115764.466714337</v>
+      </c>
+      <c r="J78">
+        <v>4842103.949121629</v>
+      </c>
+      <c r="K78">
+        <v>3987529.563501518</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79">
+        <v>708</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79">
+        <v>176.142</v>
+      </c>
+      <c r="F79">
+        <v>1116421.04355408</v>
+      </c>
+      <c r="G79">
+        <v>4841399.266768956</v>
+      </c>
+      <c r="H79">
+        <v>3986061.871253837</v>
+      </c>
+      <c r="I79">
+        <v>1115816.284923123</v>
+      </c>
+      <c r="J79">
+        <v>4842055.2975368</v>
+      </c>
+      <c r="K79">
+        <v>3987484.940246277</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80">
+        <v>708</v>
+      </c>
+      <c r="B80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80">
+        <v>177.142</v>
+      </c>
+      <c r="F80">
+        <v>1116419.365309479</v>
+      </c>
+      <c r="G80">
+        <v>4841415.779567651</v>
+      </c>
+      <c r="H80">
+        <v>3986078.959616861</v>
+      </c>
+      <c r="I80">
+        <v>1115869.379107628</v>
+      </c>
+      <c r="J80">
+        <v>4842006.64595197</v>
+      </c>
+      <c r="K80">
+        <v>3987425.168313056</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81">
+        <v>708</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81">
+        <v>178.142</v>
+      </c>
+      <c r="F81">
+        <v>1116417.821040329</v>
+      </c>
+      <c r="G81">
+        <v>4841432.292366349</v>
+      </c>
+      <c r="H81">
+        <v>3986095.126839994</v>
+      </c>
+      <c r="I81">
+        <v>1115923.780687582</v>
+      </c>
+      <c r="J81">
+        <v>4841957.994367139</v>
+      </c>
+      <c r="K81">
+        <v>3987350.247701856</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82">
+        <v>708</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82">
+        <v>179.142</v>
+      </c>
+      <c r="F82">
+        <v>1116416.393834325</v>
+      </c>
+      <c r="G82">
+        <v>4841448.805165046</v>
+      </c>
+      <c r="H82">
+        <v>3986110.467171651</v>
+      </c>
+      <c r="I82">
+        <v>1115979.521856393</v>
+      </c>
+      <c r="J82">
+        <v>4841909.34278231</v>
+      </c>
+      <c r="K82">
+        <v>3987260.178412676</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83">
+        <v>708</v>
+      </c>
+      <c r="B83" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83">
+        <v>180.142</v>
+      </c>
+      <c r="F83">
+        <v>1116415.069622444</v>
+      </c>
+      <c r="G83">
+        <v>4841465.317963742</v>
+      </c>
+      <c r="H83">
+        <v>3986125.061096679</v>
+      </c>
+      <c r="I83">
+        <v>1116036.635600206</v>
+      </c>
+      <c r="J83">
+        <v>4841860.691197481</v>
+      </c>
+      <c r="K83">
+        <v>3987154.960445516</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84">
+        <v>708</v>
+      </c>
+      <c r="B84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84">
+        <v>181.142</v>
+      </c>
+      <c r="F84">
+        <v>1116413.836592901</v>
+      </c>
+      <c r="G84">
+        <v>4841481.830762438</v>
+      </c>
+      <c r="H84">
+        <v>3986138.977892361</v>
+      </c>
+      <c r="I84">
+        <v>1116095.155717416</v>
+      </c>
+      <c r="J84">
+        <v>4841812.039612651</v>
+      </c>
+      <c r="K84">
+        <v>3987034.593800376</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85">
+        <v>708</v>
+      </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85">
+        <v>182.142</v>
+      </c>
+      <c r="F85">
+        <v>1116412.684746181</v>
+      </c>
+      <c r="G85">
+        <v>4841498.343561136</v>
+      </c>
+      <c r="H85">
+        <v>3986152.277617319</v>
+      </c>
+      <c r="I85">
+        <v>1116155.116838675</v>
+      </c>
+      <c r="J85">
+        <v>4841763.388027822</v>
+      </c>
+      <c r="K85">
+        <v>3986899.078477256</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86">
+        <v>708</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" t="s">
+        <v>14</v>
+      </c>
+      <c r="D86" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86">
+        <v>183.142</v>
+      </c>
+      <c r="F86">
+        <v>1116411.605552735</v>
+      </c>
+      <c r="G86">
+        <v>4841514.856359832</v>
+      </c>
+      <c r="H86">
+        <v>3986165.012677902</v>
+      </c>
+      <c r="I86">
+        <v>1116216.554447381</v>
+      </c>
+      <c r="J86">
+        <v>4841714.736442992</v>
+      </c>
+      <c r="K86">
+        <v>3986748.414476156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87">
+        <v>708</v>
+      </c>
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87">
+        <v>184.142</v>
+      </c>
+      <c r="F87">
+        <v>1116410.591686476</v>
+      </c>
+      <c r="G87">
+        <v>4841531.369158529</v>
+      </c>
+      <c r="H87">
+        <v>3986177.229075406</v>
+      </c>
+      <c r="I87">
+        <v>1116279.504900681</v>
+      </c>
+      <c r="J87">
+        <v>4841666.084858163</v>
+      </c>
+      <c r="K87">
+        <v>3986582.601797077</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88">
+        <v>708</v>
+      </c>
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88">
+        <v>185.142</v>
+      </c>
+      <c r="F88">
+        <v>1116409.636815014</v>
+      </c>
+      <c r="G88">
+        <v>4841547.881957225</v>
+      </c>
+      <c r="H88">
+        <v>3986188.967409092</v>
+      </c>
+      <c r="I88">
+        <v>1116344.005450979</v>
+      </c>
+      <c r="J88">
+        <v>4841617.433273333</v>
+      </c>
+      <c r="K88">
+        <v>3986401.640440017</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89">
+        <v>708</v>
+      </c>
+      <c r="B89" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89">
+        <v>186.142</v>
+      </c>
+      <c r="F89">
+        <v>1116408.735432899</v>
+      </c>
+      <c r="G89">
+        <v>4841564.394755922</v>
+      </c>
+      <c r="H89">
+        <v>3986200.26369026</v>
+      </c>
+      <c r="I89">
+        <v>1116410.094267989</v>
+      </c>
+      <c r="J89">
+        <v>4841568.781688503</v>
+      </c>
+      <c r="K89">
+        <v>3986205.530404978</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90">
+        <v>708</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" t="s">
+        <v>16</v>
+      </c>
+      <c r="E90">
+        <v>187.142</v>
+      </c>
+      <c r="F90">
+        <v>1116407.882727821</v>
+      </c>
+      <c r="G90">
+        <v>4841580.907554619</v>
+      </c>
+      <c r="H90">
+        <v>3986211.150008511</v>
+      </c>
+      <c r="I90">
+        <v>1116477.810461318</v>
+      </c>
+      <c r="J90">
+        <v>4841520.130103674</v>
+      </c>
+      <c r="K90">
+        <v>3985994.271691959</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91">
+        <v>708</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" t="s">
+        <v>16</v>
+      </c>
+      <c r="E91">
+        <v>188.142</v>
+      </c>
+      <c r="F91">
+        <v>1116407.074472343</v>
+      </c>
+      <c r="G91">
+        <v>4841597.420353315</v>
+      </c>
+      <c r="H91">
+        <v>3986221.655081299</v>
+      </c>
+      <c r="I91">
+        <v>1116547.194103609</v>
+      </c>
+      <c r="J91">
+        <v>4841471.478518845</v>
+      </c>
+      <c r="K91">
+        <v>3985767.86430096</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92">
+        <v>708</v>
+      </c>
+      <c r="B92" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" t="s">
+        <v>16</v>
+      </c>
+      <c r="E92">
+        <v>189.142</v>
+      </c>
+      <c r="F92">
+        <v>1116406.306935606</v>
+      </c>
+      <c r="G92">
+        <v>4841613.933152012</v>
+      </c>
+      <c r="H92">
+        <v>3986231.804710469</v>
+      </c>
+      <c r="I92">
+        <v>1116618.28625426</v>
+      </c>
+      <c r="J92">
+        <v>4841422.826934014</v>
+      </c>
+      <c r="K92">
+        <v>3985526.308231981</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93">
+        <v>708</v>
+      </c>
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" t="s">
+        <v>16</v>
+      </c>
+      <c r="E93">
+        <v>190.142</v>
+      </c>
+      <c r="F93">
+        <v>1116405.576810787</v>
+      </c>
+      <c r="G93">
+        <v>4841630.445950709</v>
+      </c>
+      <c r="H93">
+        <v>3986241.622164058</v>
+      </c>
+      <c r="I93">
+        <v>1116691.128983718</v>
+      </c>
+      <c r="J93">
+        <v>4841374.175349185</v>
+      </c>
+      <c r="K93">
+        <v>3985269.603485023</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94">
+        <v>708</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94">
+        <v>191.142</v>
+      </c>
+      <c r="F94">
+        <v>1116404.881155103</v>
+      </c>
+      <c r="G94">
+        <v>4841646.958749405</v>
+      </c>
+      <c r="H94">
+        <v>3986251.12849757</v>
+      </c>
+      <c r="I94">
+        <v>1116765.765398374</v>
+      </c>
+      <c r="J94">
+        <v>4841325.523764356</v>
+      </c>
+      <c r="K94">
+        <v>3984997.750060084</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95">
+        <v>708</v>
+      </c>
+      <c r="B95" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95">
+        <v>192.142</v>
+      </c>
+      <c r="F95">
+        <v>1116404.217339868</v>
+      </c>
+      <c r="G95">
+        <v>4841663.471548102</v>
+      </c>
+      <c r="H95">
+        <v>3986260.342825901</v>
+      </c>
+      <c r="I95">
+        <v>1116842.239666077</v>
+      </c>
+      <c r="J95">
+        <v>4841276.872179527</v>
+      </c>
+      <c r="K95">
+        <v>3984710.747957166</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96">
+        <v>708</v>
+      </c>
+      <c r="B96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96">
+        <v>193.142</v>
+      </c>
+      <c r="F96">
+        <v>1116403.583008677</v>
+      </c>
+      <c r="G96">
+        <v>4841679.9843468</v>
+      </c>
+      <c r="H96">
+        <v>3986269.282554722</v>
+      </c>
+      <c r="I96">
+        <v>1116920.597042267</v>
+      </c>
+      <c r="J96">
+        <v>4841228.220594697</v>
+      </c>
+      <c r="K96">
+        <v>3984408.597176268</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97">
+        <v>708</v>
+      </c>
+      <c r="B97" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" t="s">
+        <v>16</v>
+      </c>
+      <c r="E97">
+        <v>194.142</v>
+      </c>
+      <c r="F97">
+        <v>1116402.976042194</v>
+      </c>
+      <c r="G97">
+        <v>4841696.497145495</v>
+      </c>
+      <c r="H97">
+        <v>3986277.963578381</v>
+      </c>
+      <c r="I97">
+        <v>1117000.883896758</v>
+      </c>
+      <c r="J97">
+        <v>4841179.569009867</v>
+      </c>
+      <c r="K97">
+        <v>3984091.29771739</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98">
+        <v>708</v>
+      </c>
+      <c r="B98" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98">
+        <v>195.142</v>
+      </c>
+      <c r="F98">
+        <v>1116402.394528351</v>
+      </c>
+      <c r="G98">
+        <v>4841713.009944192</v>
+      </c>
+      <c r="H98">
+        <v>3986286.400449956</v>
+      </c>
+      <c r="I98">
+        <v>1117083.147741178</v>
+      </c>
+      <c r="J98">
+        <v>4841130.917425037</v>
+      </c>
+      <c r="K98">
+        <v>3983758.849580532</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99">
+        <v>708</v>
+      </c>
+      <c r="B99" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" t="s">
+        <v>16</v>
+      </c>
+      <c r="E99">
+        <v>196.142</v>
+      </c>
+      <c r="F99">
+        <v>1116401.836736999</v>
+      </c>
+      <c r="G99">
+        <v>4841729.522742888</v>
+      </c>
+      <c r="H99">
+        <v>3986294.606528055</v>
+      </c>
+      <c r="I99">
+        <v>1117167.437257086</v>
+      </c>
+      <c r="J99">
+        <v>4841082.265840207</v>
+      </c>
+      <c r="K99">
+        <v>3983411.252765695</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100">
+        <v>708</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E100">
+        <v>197.142</v>
+      </c>
+      <c r="F100">
+        <v>1116401.30109825</v>
+      </c>
+      <c r="G100">
+        <v>4841746.035541586</v>
+      </c>
+      <c r="H100">
+        <v>3986302.594104057</v>
+      </c>
+      <c r="I100">
+        <v>1117253.802324778</v>
+      </c>
+      <c r="J100">
+        <v>4841033.614255378</v>
+      </c>
+      <c r="K100">
+        <v>3983048.507272877</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101">
+        <v>708</v>
+      </c>
+      <c r="B101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" t="s">
+        <v>16</v>
+      </c>
+      <c r="E101">
+        <v>198.142</v>
+      </c>
+      <c r="F101">
+        <v>1116400.786183885</v>
+      </c>
+      <c r="G101">
+        <v>4841762.548340282</v>
+      </c>
+      <c r="H101">
+        <v>3986310.374512849</v>
+      </c>
+      <c r="I101">
+        <v>1117342.294052808</v>
+      </c>
+      <c r="J101">
+        <v>4840984.962670549</v>
+      </c>
+      <c r="K101">
+        <v>3982670.613102079</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102">
+        <v>708</v>
+      </c>
+      <c r="B102" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E102">
+        <v>199.142</v>
+      </c>
+      <c r="F102">
+        <v>1116400.290691332</v>
+      </c>
+      <c r="G102">
+        <v>4841779.061138978</v>
+      </c>
+      <c r="H102">
+        <v>3986317.958229573</v>
+      </c>
+      <c r="I102">
+        <v>1117432.96480823</v>
+      </c>
+      <c r="J102">
+        <v>4840936.31108572</v>
+      </c>
+      <c r="K102">
+        <v>3982277.570253303</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103">
+        <v>708</v>
+      </c>
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" t="s">
+        <v>16</v>
+      </c>
+      <c r="E103">
+        <v>200.142</v>
+      </c>
+      <c r="F103">
+        <v>1116399.813429808</v>
+      </c>
+      <c r="G103">
+        <v>4841795.573937675</v>
+      </c>
+      <c r="H103">
+        <v>3986325.354954425</v>
+      </c>
+      <c r="I103">
+        <v>1117525.868247588</v>
+      </c>
+      <c r="J103">
+        <v>4840887.659500889</v>
+      </c>
+      <c r="K103">
+        <v>3981869.378726545</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104">
+        <v>708</v>
+      </c>
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" t="s">
+        <v>16</v>
+      </c>
+      <c r="E104">
+        <v>201.142</v>
+      </c>
+      <c r="F104">
+        <v>1116399.353308277</v>
+      </c>
+      <c r="G104">
+        <v>4841812.086736373</v>
+      </c>
+      <c r="H104">
+        <v>3986332.573687267</v>
+      </c>
+      <c r="I104">
+        <v>1117621.059348671</v>
+      </c>
+      <c r="J104">
+        <v>4840839.007916059</v>
+      </c>
+      <c r="K104">
+        <v>3981446.038521809</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105">
+        <v>708</v>
+      </c>
+      <c r="B105" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E105">
+        <v>202.142</v>
+      </c>
+      <c r="F105">
+        <v>1116398.909324965</v>
+      </c>
+      <c r="G105">
+        <v>4841828.599535068</v>
+      </c>
+      <c r="H105">
+        <v>3986339.622793457</v>
+      </c>
+      <c r="I105">
+        <v>1117718.594443044</v>
+      </c>
+      <c r="J105">
+        <v>4840790.35633123</v>
+      </c>
+      <c r="K105">
+        <v>3981007.549639091</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106">
+        <v>708</v>
+      </c>
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" t="s">
+        <v>16</v>
+      </c>
+      <c r="E106">
+        <v>203.142</v>
+      </c>
+      <c r="F106">
+        <v>1116398.480558181</v>
+      </c>
+      <c r="G106">
+        <v>4841845.112333765</v>
+      </c>
+      <c r="H106">
+        <v>3986346.510062131</v>
+      </c>
+      <c r="I106">
+        <v>1117818.531249385</v>
+      </c>
+      <c r="J106">
+        <v>4840741.704746401</v>
+      </c>
+      <c r="K106">
+        <v>3980553.912078395</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107">
+        <v>708</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" t="s">
+        <v>16</v>
+      </c>
+      <c r="E107">
+        <v>204.142</v>
+      </c>
+      <c r="F107">
+        <v>1116398.066158276</v>
+      </c>
+      <c r="G107">
+        <v>4841861.625132462</v>
+      </c>
+      <c r="H107">
+        <v>3986353.242757936</v>
+      </c>
+      <c r="I107">
+        <v>1117920.928907642</v>
+      </c>
+      <c r="J107">
+        <v>4840693.053161571</v>
+      </c>
+      <c r="K107">
+        <v>3980085.125839719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>